<commit_message>
Adaption during paper acceptance
</commit_message>
<xml_diff>
--- a/02_Energy_calculation/03 Inefficiencies and scaled energy.xlsx
+++ b/02_Energy_calculation/03 Inefficiencies and scaled energy.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29231"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="N:\Projekte\ETSAP - Follow\05 Reports\03 Veröffentlichungen\01 Material und Energienachfragen\GitHub\Industrial-energy-demands\02_Energy_calculation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ge37kog\bwSyncShare\Follow ETSAP\Veröffentlichungen\Materials and energy demands 2018\Publication\ANNEX_submission\02_Energy_calculation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB9C88A6-9C45-4EA1-AC9C-A164D0E28820}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FDDF7E0E-38C6-4047-9FD6-C20A04829644}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="180" windowWidth="29040" windowHeight="17520" tabRatio="500" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Info" sheetId="7" r:id="rId1"/>
@@ -340,7 +340,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="419" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="423" uniqueCount="98">
   <si>
     <t>Calculated BAT energy demand</t>
   </si>
@@ -2189,9 +2189,6 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center"/>
-    </xf>
     <xf numFmtId="169" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="center"/>
     </xf>
@@ -2311,6 +2308,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="6">
@@ -5814,7 +5814,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Chemicals!$AJ$2</c:f>
+              <c:f>Chemicals!$AN$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -5849,7 +5849,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{D85D874B-4A15-47B6-81ED-579C3F65AA08}" type="CELLRANGE">
+                    <a:fld id="{E92E0D10-6F4A-4C46-A417-D5E4823CFA26}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[ZELLBEREICH]</a:t>
@@ -5899,7 +5899,7 @@
                         <a:cs typeface="+mn-cs"/>
                       </a:defRPr>
                     </a:pPr>
-                    <a:fld id="{A500307B-C192-41E2-A334-62069ECE93B9}" type="CELLRANGE">
+                    <a:fld id="{924D1EB1-188E-4857-B5CC-90A22BBD3270}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr>
                         <a:defRPr>
@@ -5975,7 +5975,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{C0ECB066-445C-4FF7-9ABB-B9529C15F4FE}" type="CELLRANGE">
+                    <a:fld id="{629461C2-AD98-4909-849A-A1B1DAA56E4F}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[ZELLBEREICH]</a:t>
@@ -6013,7 +6013,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{E5722BDA-1027-47A2-AD08-0636A2F66143}" type="CELLRANGE">
+                    <a:fld id="{5E4F3521-3EB7-4B99-B9F4-FE5A00F35CC7}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[ZELLBEREICH]</a:t>
@@ -6051,7 +6051,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{DE532313-3A5C-43C5-BC74-6D633D8FB2BB}" type="CELLRANGE">
+                    <a:fld id="{FB07C9D9-44B1-44F0-B296-2AEECBC99300}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[ZELLBEREICH]</a:t>
@@ -6089,7 +6089,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{F330A20B-57F9-494B-B323-9ABC80CFA243}" type="CELLRANGE">
+                    <a:fld id="{4F2BBC6F-1FCA-4DF0-9632-0594D6753995}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[ZELLBEREICH]</a:t>
@@ -6127,7 +6127,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{54D37DB4-BDAF-4B1D-A4F9-32E870A6CACD}" type="CELLRANGE">
+                    <a:fld id="{88D2CE80-DC06-488A-9744-A02C1967F0C2}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[ZELLBEREICH]</a:t>
@@ -6251,7 +6251,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{FFB3094B-3AE7-4AAA-A5E0-A71838770D4B}" type="CELLRANGE">
+                    <a:fld id="{1104165D-580A-4680-A8A8-34202CEF82B4}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[ZELLBEREICH]</a:t>
@@ -6289,7 +6289,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{C22FEDED-F875-49BE-9F2F-1EEC6ABA51BA}" type="CELLRANGE">
+                    <a:fld id="{93B705BB-4DC8-447D-8A22-02CF24B48668}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[ZELLBEREICH]</a:t>
@@ -6327,7 +6327,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{4DC1C966-92FD-4BFD-8379-0C31914E97AF}" type="CELLRANGE">
+                    <a:fld id="{F523AE8F-CCA2-42AC-9CE1-6E5973947B11}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[ZELLBEREICH]</a:t>
@@ -6365,7 +6365,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{84485B03-3980-4A90-9F25-FBDA9C236F5B}" type="CELLRANGE">
+                    <a:fld id="{B57B3B14-483C-4975-A2BB-42236BB99772}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[ZELLBEREICH]</a:t>
@@ -6489,7 +6489,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{450ED768-6457-4FCC-B068-1A366F438598}" type="CELLRANGE">
+                    <a:fld id="{69FCF886-E393-4A49-BABC-631101D6A844}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[ZELLBEREICH]</a:t>
@@ -6539,7 +6539,7 @@
                         <a:cs typeface="+mn-cs"/>
                       </a:defRPr>
                     </a:pPr>
-                    <a:fld id="{964F211E-1783-41DA-AF29-DF9B66583E18}" type="CELLRANGE">
+                    <a:fld id="{1B355111-47F3-4A8F-851A-1458F82EAF84}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr>
                         <a:defRPr>
@@ -6697,7 +6697,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>(Chemicals!$AJ$5:$AJ$7,Chemicals!$AJ$9:$AJ$20)</c:f>
+              <c:f>(Chemicals!$AN$5:$AN$7,Chemicals!$AN$9:$AN$20)</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="15"/>
@@ -6752,7 +6752,7 @@
           <c:extLst>
             <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
               <c15:datalabelsRange>
-                <c15:f>(Chemicals!$AI$5:$AI$7,Chemicals!$AI$9:$AI$20)</c15:f>
+                <c15:f>(Chemicals!$AM$5:$AM$7,Chemicals!$AM$9:$AM$20)</c15:f>
                 <c15:dlblRangeCache>
                   <c:ptCount val="15"/>
                   <c:pt idx="0">
@@ -6813,7 +6813,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Chemicals!$AK$2</c:f>
+              <c:f>Chemicals!$AO$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -6892,7 +6892,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>(Chemicals!$AK$5:$AK$7,Chemicals!$AK$9:$AK$20)</c:f>
+              <c:f>(Chemicals!$AO$5:$AO$7,Chemicals!$AO$9:$AO$20)</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="15"/>
@@ -6955,7 +6955,7 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>Chemicals!$AL$2</c:f>
+              <c:f>Chemicals!$AP$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -7034,7 +7034,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>(Chemicals!$AL$5:$AL$7,Chemicals!$AL$9:$AL$20)</c:f>
+              <c:f>(Chemicals!$AP$5:$AP$7,Chemicals!$AP$9:$AP$20)</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="15"/>
@@ -7275,7 +7275,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Chemicals!$AJ$2</c:f>
+              <c:f>Chemicals!$AN$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -7309,7 +7309,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Chemicals!$AJ$8</c:f>
+              <c:f>Chemicals!$AN$8</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="1"/>
@@ -7330,7 +7330,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Chemicals!$AK$2</c:f>
+              <c:f>Chemicals!$AO$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -7364,7 +7364,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Chemicals!$AK$8</c:f>
+              <c:f>Chemicals!$AO$8</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="1"/>
@@ -7385,7 +7385,7 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>Chemicals!$AL$2</c:f>
+              <c:f>Chemicals!$AP$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -7432,7 +7432,7 @@
                         <a:cs typeface="+mn-cs"/>
                       </a:defRPr>
                     </a:pPr>
-                    <a:fld id="{902A5140-B312-41BC-847D-0095DA4B9E91}" type="CELLRANGE">
+                    <a:fld id="{47B50B6E-32E8-4769-9C38-96975C3592B8}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr>
                         <a:defRPr/>
@@ -7560,7 +7560,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Chemicals!$AL$8</c:f>
+              <c:f>Chemicals!$AP$8</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="1"/>
@@ -7573,7 +7573,7 @@
           <c:extLst>
             <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
               <c15:datalabelsRange>
-                <c15:f>Chemicals!$AI$8</c15:f>
+                <c15:f>Chemicals!$AM$8</c15:f>
                 <c15:dlblRangeCache>
                   <c:ptCount val="1"/>
                   <c:pt idx="0">
@@ -7777,7 +7777,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Chemicals!$AC$2</c:f>
+              <c:f>Chemicals!$AG$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -7856,7 +7856,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Chemicals!$AC$5:$AC$20</c:f>
+              <c:f>Chemicals!$AG$5:$AG$20</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="16"/>
@@ -7922,7 +7922,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Chemicals!$AD$2</c:f>
+              <c:f>Chemicals!$AH$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -8001,7 +8001,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Chemicals!$AD$5:$AD$20</c:f>
+              <c:f>Chemicals!$AH$5:$AH$20</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="16"/>
@@ -8067,7 +8067,7 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>Chemicals!$AE$2</c:f>
+              <c:f>Chemicals!$AI$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -8146,7 +8146,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Chemicals!$AE$5:$AE$20</c:f>
+              <c:f>Chemicals!$AI$5:$AI$20</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="16"/>
@@ -8212,7 +8212,7 @@
           <c:order val="3"/>
           <c:tx>
             <c:strRef>
-              <c:f>Chemicals!$AF$2</c:f>
+              <c:f>Chemicals!$AJ$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -8291,7 +8291,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Chemicals!$AF$5:$AF$20</c:f>
+              <c:f>Chemicals!$AJ$5:$AJ$20</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="16"/>
@@ -8357,7 +8357,7 @@
           <c:order val="4"/>
           <c:tx>
             <c:strRef>
-              <c:f>Chemicals!$AG$2</c:f>
+              <c:f>Chemicals!$AK$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -8436,7 +8436,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Chemicals!$AG$5:$AG$20</c:f>
+              <c:f>Chemicals!$AK$5:$AK$20</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="16"/>
@@ -8502,7 +8502,7 @@
           <c:order val="5"/>
           <c:tx>
             <c:strRef>
-              <c:f>Chemicals!$AH$2</c:f>
+              <c:f>Chemicals!$AL$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -8581,7 +8581,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Chemicals!$AH$5:$AH$20</c:f>
+              <c:f>Chemicals!$AL$5:$AL$20</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="16"/>
@@ -24347,13 +24347,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>29</xdr:col>
+      <xdr:col>33</xdr:col>
       <xdr:colOff>419978</xdr:colOff>
       <xdr:row>28</xdr:row>
       <xdr:rowOff>67560</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>37</xdr:col>
+      <xdr:col>41</xdr:col>
       <xdr:colOff>75132</xdr:colOff>
       <xdr:row>35</xdr:row>
       <xdr:rowOff>120450</xdr:rowOff>
@@ -25576,7 +25576,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5A5F30B7-898F-4227-87DD-7236F1372F46}">
   <dimension ref="A1:A24"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+    <sheetView showGridLines="0" workbookViewId="0">
       <selection activeCell="A19" sqref="A19"/>
     </sheetView>
   </sheetViews>
@@ -25708,42 +25708,42 @@
   <sheetData>
     <row r="1" spans="1:34" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="93"/>
-      <c r="B1" s="235" t="s">
+      <c r="B1" s="234" t="s">
         <v>55</v>
       </c>
-      <c r="C1" s="236"/>
-      <c r="D1" s="236"/>
-      <c r="E1" s="236"/>
-      <c r="F1" s="242" t="s">
+      <c r="C1" s="235"/>
+      <c r="D1" s="235"/>
+      <c r="E1" s="235"/>
+      <c r="F1" s="241" t="s">
         <v>0</v>
       </c>
-      <c r="G1" s="240"/>
-      <c r="H1" s="240"/>
-      <c r="I1" s="240"/>
-      <c r="J1" s="240"/>
-      <c r="K1" s="241"/>
-      <c r="L1" s="240" t="s">
+      <c r="G1" s="239"/>
+      <c r="H1" s="239"/>
+      <c r="I1" s="239"/>
+      <c r="J1" s="239"/>
+      <c r="K1" s="240"/>
+      <c r="L1" s="239" t="s">
         <v>60</v>
       </c>
-      <c r="M1" s="240"/>
-      <c r="N1" s="240"/>
-      <c r="O1" s="240"/>
-      <c r="P1" s="240"/>
-      <c r="Q1" s="240"/>
-      <c r="R1" s="240"/>
-      <c r="S1" s="241"/>
-      <c r="T1" s="243" t="s">
+      <c r="M1" s="239"/>
+      <c r="N1" s="239"/>
+      <c r="O1" s="239"/>
+      <c r="P1" s="239"/>
+      <c r="Q1" s="239"/>
+      <c r="R1" s="239"/>
+      <c r="S1" s="240"/>
+      <c r="T1" s="242" t="s">
         <v>89</v>
       </c>
-      <c r="U1" s="244"/>
-      <c r="V1" s="244"/>
-      <c r="W1" s="244"/>
-      <c r="X1" s="244"/>
-      <c r="Y1" s="245"/>
-      <c r="Z1" s="233" t="s">
+      <c r="U1" s="243"/>
+      <c r="V1" s="243"/>
+      <c r="W1" s="243"/>
+      <c r="X1" s="243"/>
+      <c r="Y1" s="244"/>
+      <c r="Z1" s="232" t="s">
         <v>93</v>
       </c>
-      <c r="AA1" s="234"/>
+      <c r="AA1" s="233"/>
     </row>
     <row r="2" spans="1:34" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="94" t="s">
@@ -25785,16 +25785,16 @@
       <c r="M2" s="83" t="s">
         <v>57</v>
       </c>
-      <c r="N2" s="248" t="s">
+      <c r="N2" s="247" t="s">
         <v>58</v>
       </c>
-      <c r="O2" s="249"/>
-      <c r="P2" s="250"/>
-      <c r="Q2" s="249" t="s">
+      <c r="O2" s="248"/>
+      <c r="P2" s="249"/>
+      <c r="Q2" s="248" t="s">
         <v>59</v>
       </c>
-      <c r="R2" s="249"/>
-      <c r="S2" s="251"/>
+      <c r="R2" s="248"/>
+      <c r="S2" s="250"/>
       <c r="T2" s="3" t="s">
         <v>44</v>
       </c>
@@ -25869,48 +25869,48 @@
       <c r="A4" s="95" t="s">
         <v>7</v>
       </c>
-      <c r="B4" s="237" t="s">
+      <c r="B4" s="236" t="s">
         <v>8</v>
       </c>
-      <c r="C4" s="238"/>
-      <c r="D4" s="238"/>
-      <c r="E4" s="239"/>
-      <c r="F4" s="246" t="s">
+      <c r="C4" s="237"/>
+      <c r="D4" s="237"/>
+      <c r="E4" s="238"/>
+      <c r="F4" s="245" t="s">
         <v>8</v>
       </c>
-      <c r="G4" s="238"/>
-      <c r="H4" s="238"/>
-      <c r="I4" s="238"/>
-      <c r="J4" s="238"/>
-      <c r="K4" s="238"/>
+      <c r="G4" s="237"/>
+      <c r="H4" s="237"/>
+      <c r="I4" s="237"/>
+      <c r="J4" s="237"/>
+      <c r="K4" s="237"/>
       <c r="L4" s="79" t="s">
         <v>9</v>
       </c>
       <c r="M4" s="82" t="s">
         <v>9</v>
       </c>
-      <c r="N4" s="252" t="s">
+      <c r="N4" s="251" t="s">
         <v>9</v>
       </c>
-      <c r="O4" s="239"/>
-      <c r="P4" s="239"/>
-      <c r="Q4" s="242" t="s">
+      <c r="O4" s="238"/>
+      <c r="P4" s="238"/>
+      <c r="Q4" s="241" t="s">
         <v>9</v>
       </c>
-      <c r="R4" s="240"/>
-      <c r="S4" s="240"/>
-      <c r="T4" s="247" t="s">
+      <c r="R4" s="239"/>
+      <c r="S4" s="239"/>
+      <c r="T4" s="246" t="s">
         <v>8</v>
       </c>
-      <c r="U4" s="247"/>
-      <c r="V4" s="247"/>
-      <c r="W4" s="247"/>
-      <c r="X4" s="247"/>
-      <c r="Y4" s="247"/>
-      <c r="Z4" s="253" t="s">
+      <c r="U4" s="246"/>
+      <c r="V4" s="246"/>
+      <c r="W4" s="246"/>
+      <c r="X4" s="246"/>
+      <c r="Y4" s="246"/>
+      <c r="Z4" s="252" t="s">
         <v>8</v>
       </c>
-      <c r="AA4" s="254"/>
+      <c r="AA4" s="253"/>
     </row>
     <row r="5" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A5" s="50" t="s">
@@ -27583,48 +27583,48 @@
   <sheetData>
     <row r="1" spans="1:39" ht="63" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="9"/>
-      <c r="B1" s="256" t="s">
+      <c r="B1" s="255" t="s">
         <v>55</v>
       </c>
-      <c r="C1" s="256"/>
-      <c r="D1" s="256"/>
-      <c r="E1" s="256"/>
-      <c r="F1" s="256"/>
-      <c r="G1" s="256"/>
-      <c r="H1" s="258" t="s">
+      <c r="C1" s="255"/>
+      <c r="D1" s="255"/>
+      <c r="E1" s="255"/>
+      <c r="F1" s="255"/>
+      <c r="G1" s="255"/>
+      <c r="H1" s="257" t="s">
         <v>0</v>
       </c>
-      <c r="I1" s="258"/>
-      <c r="J1" s="258"/>
-      <c r="K1" s="258"/>
-      <c r="L1" s="258"/>
-      <c r="M1" s="258"/>
-      <c r="N1" s="258"/>
-      <c r="O1" s="258"/>
-      <c r="P1" s="242" t="s">
+      <c r="I1" s="257"/>
+      <c r="J1" s="257"/>
+      <c r="K1" s="257"/>
+      <c r="L1" s="257"/>
+      <c r="M1" s="257"/>
+      <c r="N1" s="257"/>
+      <c r="O1" s="257"/>
+      <c r="P1" s="241" t="s">
         <v>60</v>
       </c>
-      <c r="Q1" s="240"/>
-      <c r="R1" s="240"/>
-      <c r="S1" s="240"/>
-      <c r="T1" s="240"/>
-      <c r="U1" s="240"/>
-      <c r="V1" s="240"/>
-      <c r="W1" s="241"/>
-      <c r="X1" s="255" t="s">
+      <c r="Q1" s="239"/>
+      <c r="R1" s="239"/>
+      <c r="S1" s="239"/>
+      <c r="T1" s="239"/>
+      <c r="U1" s="239"/>
+      <c r="V1" s="239"/>
+      <c r="W1" s="240"/>
+      <c r="X1" s="254" t="s">
         <v>89</v>
       </c>
-      <c r="Y1" s="255"/>
-      <c r="Z1" s="255"/>
-      <c r="AA1" s="255"/>
-      <c r="AB1" s="255"/>
-      <c r="AC1" s="255"/>
-      <c r="AD1" s="255"/>
-      <c r="AE1" s="255"/>
-      <c r="AF1" s="233" t="s">
+      <c r="Y1" s="254"/>
+      <c r="Z1" s="254"/>
+      <c r="AA1" s="254"/>
+      <c r="AB1" s="254"/>
+      <c r="AC1" s="254"/>
+      <c r="AD1" s="254"/>
+      <c r="AE1" s="254"/>
+      <c r="AF1" s="232" t="s">
         <v>93</v>
       </c>
-      <c r="AG1" s="234"/>
+      <c r="AG1" s="233"/>
     </row>
     <row r="2" spans="1:39" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="10" t="s">
@@ -27678,16 +27678,16 @@
       <c r="Q2" s="83" t="s">
         <v>57</v>
       </c>
-      <c r="R2" s="248" t="s">
+      <c r="R2" s="247" t="s">
         <v>58</v>
       </c>
-      <c r="S2" s="249"/>
-      <c r="T2" s="250"/>
-      <c r="U2" s="249" t="s">
+      <c r="S2" s="248"/>
+      <c r="T2" s="249"/>
+      <c r="U2" s="248" t="s">
         <v>59</v>
       </c>
-      <c r="V2" s="249"/>
-      <c r="W2" s="251"/>
+      <c r="V2" s="248"/>
+      <c r="W2" s="250"/>
       <c r="X2" s="3" t="s">
         <v>26</v>
       </c>
@@ -27774,54 +27774,54 @@
       <c r="A4" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="B4" s="257" t="s">
+      <c r="B4" s="256" t="s">
         <v>8</v>
       </c>
-      <c r="C4" s="257"/>
-      <c r="D4" s="257"/>
-      <c r="E4" s="257"/>
-      <c r="F4" s="257"/>
-      <c r="G4" s="257"/>
-      <c r="H4" s="246" t="s">
+      <c r="C4" s="256"/>
+      <c r="D4" s="256"/>
+      <c r="E4" s="256"/>
+      <c r="F4" s="256"/>
+      <c r="G4" s="256"/>
+      <c r="H4" s="245" t="s">
         <v>8</v>
       </c>
-      <c r="I4" s="246"/>
-      <c r="J4" s="246"/>
-      <c r="K4" s="246"/>
-      <c r="L4" s="246"/>
-      <c r="M4" s="246"/>
-      <c r="N4" s="246"/>
-      <c r="O4" s="246"/>
+      <c r="I4" s="245"/>
+      <c r="J4" s="245"/>
+      <c r="K4" s="245"/>
+      <c r="L4" s="245"/>
+      <c r="M4" s="245"/>
+      <c r="N4" s="245"/>
+      <c r="O4" s="245"/>
       <c r="P4" s="82" t="s">
         <v>9</v>
       </c>
       <c r="Q4" s="82" t="s">
         <v>9</v>
       </c>
-      <c r="R4" s="252" t="s">
+      <c r="R4" s="251" t="s">
         <v>9</v>
       </c>
-      <c r="S4" s="239"/>
-      <c r="T4" s="239"/>
-      <c r="U4" s="252" t="s">
+      <c r="S4" s="238"/>
+      <c r="T4" s="238"/>
+      <c r="U4" s="251" t="s">
         <v>9</v>
       </c>
-      <c r="V4" s="239"/>
-      <c r="W4" s="239"/>
-      <c r="X4" s="247" t="s">
+      <c r="V4" s="238"/>
+      <c r="W4" s="238"/>
+      <c r="X4" s="246" t="s">
         <v>8</v>
       </c>
-      <c r="Y4" s="247"/>
-      <c r="Z4" s="247"/>
-      <c r="AA4" s="247"/>
-      <c r="AB4" s="247"/>
-      <c r="AC4" s="247"/>
-      <c r="AD4" s="247"/>
-      <c r="AE4" s="247"/>
-      <c r="AF4" s="253" t="s">
+      <c r="Y4" s="246"/>
+      <c r="Z4" s="246"/>
+      <c r="AA4" s="246"/>
+      <c r="AB4" s="246"/>
+      <c r="AC4" s="246"/>
+      <c r="AD4" s="246"/>
+      <c r="AE4" s="246"/>
+      <c r="AF4" s="252" t="s">
         <v>8</v>
       </c>
-      <c r="AG4" s="254"/>
+      <c r="AG4" s="253"/>
     </row>
     <row r="5" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A5" s="87" t="s">
@@ -29696,45 +29696,45 @@
   <sheetData>
     <row r="1" spans="1:36" ht="33.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="9"/>
-      <c r="B1" s="258" t="s">
+      <c r="B1" s="257" t="s">
         <v>55</v>
       </c>
-      <c r="C1" s="258"/>
-      <c r="D1" s="258"/>
-      <c r="E1" s="258"/>
-      <c r="F1" s="258"/>
-      <c r="G1" s="258" t="s">
+      <c r="C1" s="257"/>
+      <c r="D1" s="257"/>
+      <c r="E1" s="257"/>
+      <c r="F1" s="257"/>
+      <c r="G1" s="257" t="s">
         <v>0</v>
       </c>
-      <c r="H1" s="258"/>
-      <c r="I1" s="258"/>
-      <c r="J1" s="258"/>
-      <c r="K1" s="258"/>
-      <c r="L1" s="258"/>
-      <c r="M1" s="258"/>
-      <c r="N1" s="242" t="s">
+      <c r="H1" s="257"/>
+      <c r="I1" s="257"/>
+      <c r="J1" s="257"/>
+      <c r="K1" s="257"/>
+      <c r="L1" s="257"/>
+      <c r="M1" s="257"/>
+      <c r="N1" s="241" t="s">
         <v>60</v>
       </c>
-      <c r="O1" s="240"/>
-      <c r="P1" s="240"/>
-      <c r="Q1" s="240"/>
-      <c r="R1" s="240"/>
-      <c r="S1" s="240"/>
-      <c r="T1" s="240"/>
-      <c r="U1" s="241"/>
-      <c r="V1" s="255" t="s">
+      <c r="O1" s="239"/>
+      <c r="P1" s="239"/>
+      <c r="Q1" s="239"/>
+      <c r="R1" s="239"/>
+      <c r="S1" s="239"/>
+      <c r="T1" s="239"/>
+      <c r="U1" s="240"/>
+      <c r="V1" s="254" t="s">
         <v>89</v>
       </c>
-      <c r="W1" s="255"/>
-      <c r="X1" s="255"/>
-      <c r="Y1" s="255"/>
-      <c r="Z1" s="255"/>
-      <c r="AA1" s="255"/>
-      <c r="AB1" s="255"/>
-      <c r="AC1" s="233" t="s">
+      <c r="W1" s="254"/>
+      <c r="X1" s="254"/>
+      <c r="Y1" s="254"/>
+      <c r="Z1" s="254"/>
+      <c r="AA1" s="254"/>
+      <c r="AB1" s="254"/>
+      <c r="AC1" s="232" t="s">
         <v>93</v>
       </c>
-      <c r="AD1" s="234"/>
+      <c r="AD1" s="233"/>
     </row>
     <row r="2" spans="1:36" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
@@ -29782,16 +29782,16 @@
       <c r="O2" s="83" t="s">
         <v>57</v>
       </c>
-      <c r="P2" s="248" t="s">
+      <c r="P2" s="247" t="s">
         <v>58</v>
       </c>
-      <c r="Q2" s="249"/>
-      <c r="R2" s="250"/>
-      <c r="S2" s="249" t="s">
+      <c r="Q2" s="248"/>
+      <c r="R2" s="249"/>
+      <c r="S2" s="248" t="s">
         <v>59</v>
       </c>
-      <c r="T2" s="249"/>
-      <c r="U2" s="251"/>
+      <c r="T2" s="248"/>
+      <c r="U2" s="250"/>
       <c r="V2" s="25" t="s">
         <v>31</v>
       </c>
@@ -29872,51 +29872,51 @@
       <c r="A4" s="26" t="s">
         <v>7</v>
       </c>
-      <c r="B4" s="242" t="s">
+      <c r="B4" s="241" t="s">
         <v>8</v>
       </c>
-      <c r="C4" s="240"/>
-      <c r="D4" s="240"/>
-      <c r="E4" s="240"/>
-      <c r="F4" s="259"/>
-      <c r="G4" s="240" t="s">
+      <c r="C4" s="239"/>
+      <c r="D4" s="239"/>
+      <c r="E4" s="239"/>
+      <c r="F4" s="258"/>
+      <c r="G4" s="239" t="s">
         <v>8</v>
       </c>
-      <c r="H4" s="240"/>
-      <c r="I4" s="240"/>
-      <c r="J4" s="240"/>
-      <c r="K4" s="240"/>
-      <c r="L4" s="240"/>
-      <c r="M4" s="240"/>
+      <c r="H4" s="239"/>
+      <c r="I4" s="239"/>
+      <c r="J4" s="239"/>
+      <c r="K4" s="239"/>
+      <c r="L4" s="239"/>
+      <c r="M4" s="239"/>
       <c r="N4" s="196" t="s">
         <v>9</v>
       </c>
       <c r="O4" s="196" t="s">
         <v>9</v>
       </c>
-      <c r="P4" s="242" t="s">
+      <c r="P4" s="241" t="s">
         <v>9</v>
       </c>
-      <c r="Q4" s="240"/>
-      <c r="R4" s="240"/>
-      <c r="S4" s="242" t="s">
+      <c r="Q4" s="239"/>
+      <c r="R4" s="239"/>
+      <c r="S4" s="241" t="s">
         <v>9</v>
       </c>
-      <c r="T4" s="240"/>
-      <c r="U4" s="240"/>
-      <c r="V4" s="255" t="s">
+      <c r="T4" s="239"/>
+      <c r="U4" s="239"/>
+      <c r="V4" s="254" t="s">
         <v>8</v>
       </c>
-      <c r="W4" s="255"/>
-      <c r="X4" s="255"/>
-      <c r="Y4" s="255"/>
-      <c r="Z4" s="255"/>
-      <c r="AA4" s="255"/>
-      <c r="AB4" s="255"/>
-      <c r="AC4" s="253" t="s">
+      <c r="W4" s="254"/>
+      <c r="X4" s="254"/>
+      <c r="Y4" s="254"/>
+      <c r="Z4" s="254"/>
+      <c r="AA4" s="254"/>
+      <c r="AB4" s="254"/>
+      <c r="AC4" s="252" t="s">
         <v>8</v>
       </c>
-      <c r="AD4" s="254"/>
+      <c r="AD4" s="253"/>
     </row>
     <row r="5" spans="1:36" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="9" t="s">
@@ -31819,51 +31819,51 @@
   <sheetData>
     <row r="1" spans="1:43" ht="29.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1"/>
-      <c r="B1" s="242" t="s">
+      <c r="B1" s="241" t="s">
         <v>55</v>
       </c>
-      <c r="C1" s="240"/>
-      <c r="D1" s="259"/>
-      <c r="E1" s="240" t="s">
+      <c r="C1" s="239"/>
+      <c r="D1" s="258"/>
+      <c r="E1" s="239" t="s">
         <v>0</v>
       </c>
-      <c r="F1" s="240"/>
-      <c r="G1" s="240"/>
-      <c r="H1" s="240"/>
-      <c r="I1" s="240"/>
-      <c r="J1" s="240"/>
-      <c r="K1" s="240"/>
-      <c r="L1" s="240"/>
-      <c r="M1" s="240"/>
-      <c r="N1" s="240"/>
-      <c r="O1" s="240"/>
-      <c r="P1" s="240"/>
-      <c r="Q1" s="242" t="s">
+      <c r="F1" s="239"/>
+      <c r="G1" s="239"/>
+      <c r="H1" s="239"/>
+      <c r="I1" s="239"/>
+      <c r="J1" s="239"/>
+      <c r="K1" s="239"/>
+      <c r="L1" s="239"/>
+      <c r="M1" s="239"/>
+      <c r="N1" s="239"/>
+      <c r="O1" s="239"/>
+      <c r="P1" s="239"/>
+      <c r="Q1" s="241" t="s">
         <v>60</v>
       </c>
-      <c r="R1" s="240"/>
-      <c r="S1" s="240"/>
-      <c r="T1" s="240"/>
-      <c r="U1" s="240"/>
-      <c r="V1" s="240"/>
-      <c r="W1" s="240"/>
-      <c r="X1" s="241"/>
-      <c r="Y1" s="255" t="s">
+      <c r="R1" s="239"/>
+      <c r="S1" s="239"/>
+      <c r="T1" s="239"/>
+      <c r="U1" s="239"/>
+      <c r="V1" s="239"/>
+      <c r="W1" s="239"/>
+      <c r="X1" s="240"/>
+      <c r="Y1" s="254" t="s">
         <v>89</v>
       </c>
-      <c r="Z1" s="255"/>
-      <c r="AA1" s="255"/>
-      <c r="AB1" s="255"/>
-      <c r="AC1" s="255"/>
-      <c r="AD1" s="255"/>
-      <c r="AE1" s="255"/>
-      <c r="AF1" s="255"/>
-      <c r="AG1" s="255"/>
-      <c r="AH1" s="255"/>
-      <c r="AI1" s="233" t="s">
+      <c r="Z1" s="254"/>
+      <c r="AA1" s="254"/>
+      <c r="AB1" s="254"/>
+      <c r="AC1" s="254"/>
+      <c r="AD1" s="254"/>
+      <c r="AE1" s="254"/>
+      <c r="AF1" s="254"/>
+      <c r="AG1" s="254"/>
+      <c r="AH1" s="254"/>
+      <c r="AI1" s="232" t="s">
         <v>93</v>
       </c>
-      <c r="AJ1" s="234"/>
+      <c r="AJ1" s="233"/>
     </row>
     <row r="2" spans="1:43" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
@@ -31920,16 +31920,16 @@
       <c r="R2" s="83" t="s">
         <v>57</v>
       </c>
-      <c r="S2" s="248" t="s">
+      <c r="S2" s="247" t="s">
         <v>58</v>
       </c>
-      <c r="T2" s="249"/>
-      <c r="U2" s="250"/>
-      <c r="V2" s="249" t="s">
+      <c r="T2" s="248"/>
+      <c r="U2" s="249"/>
+      <c r="V2" s="248" t="s">
         <v>59</v>
       </c>
-      <c r="W2" s="249"/>
-      <c r="X2" s="251"/>
+      <c r="W2" s="248"/>
+      <c r="X2" s="250"/>
       <c r="Y2" s="11" t="s">
         <v>78</v>
       </c>
@@ -32025,57 +32025,57 @@
       <c r="A4" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="B4" s="246" t="s">
+      <c r="B4" s="245" t="s">
         <v>8</v>
       </c>
-      <c r="C4" s="238"/>
-      <c r="D4" s="260"/>
-      <c r="E4" s="238" t="s">
+      <c r="C4" s="237"/>
+      <c r="D4" s="259"/>
+      <c r="E4" s="237" t="s">
         <v>8</v>
       </c>
-      <c r="F4" s="238"/>
-      <c r="G4" s="238"/>
-      <c r="H4" s="238"/>
-      <c r="I4" s="238"/>
-      <c r="J4" s="238"/>
-      <c r="K4" s="238"/>
-      <c r="L4" s="238"/>
-      <c r="M4" s="238"/>
-      <c r="N4" s="238"/>
-      <c r="O4" s="238"/>
-      <c r="P4" s="238"/>
+      <c r="F4" s="237"/>
+      <c r="G4" s="237"/>
+      <c r="H4" s="237"/>
+      <c r="I4" s="237"/>
+      <c r="J4" s="237"/>
+      <c r="K4" s="237"/>
+      <c r="L4" s="237"/>
+      <c r="M4" s="237"/>
+      <c r="N4" s="237"/>
+      <c r="O4" s="237"/>
+      <c r="P4" s="237"/>
       <c r="Q4" s="82" t="s">
         <v>9</v>
       </c>
       <c r="R4" s="82" t="s">
         <v>9</v>
       </c>
-      <c r="S4" s="252" t="s">
+      <c r="S4" s="251" t="s">
         <v>9</v>
       </c>
-      <c r="T4" s="239"/>
-      <c r="U4" s="239"/>
-      <c r="V4" s="252" t="s">
+      <c r="T4" s="238"/>
+      <c r="U4" s="238"/>
+      <c r="V4" s="251" t="s">
         <v>9</v>
       </c>
-      <c r="W4" s="239"/>
-      <c r="X4" s="239"/>
-      <c r="Y4" s="255" t="s">
+      <c r="W4" s="238"/>
+      <c r="X4" s="238"/>
+      <c r="Y4" s="254" t="s">
         <v>8</v>
       </c>
-      <c r="Z4" s="255"/>
-      <c r="AA4" s="255"/>
-      <c r="AB4" s="255"/>
-      <c r="AC4" s="255"/>
-      <c r="AD4" s="255"/>
-      <c r="AE4" s="255"/>
-      <c r="AF4" s="255"/>
-      <c r="AG4" s="255"/>
-      <c r="AH4" s="255"/>
-      <c r="AI4" s="253" t="s">
+      <c r="Z4" s="254"/>
+      <c r="AA4" s="254"/>
+      <c r="AB4" s="254"/>
+      <c r="AC4" s="254"/>
+      <c r="AD4" s="254"/>
+      <c r="AE4" s="254"/>
+      <c r="AF4" s="254"/>
+      <c r="AG4" s="254"/>
+      <c r="AH4" s="254"/>
+      <c r="AI4" s="252" t="s">
         <v>8</v>
       </c>
-      <c r="AJ4" s="254"/>
+      <c r="AJ4" s="253"/>
     </row>
     <row r="5" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A5" s="44" t="s">
@@ -34301,12 +34301,6 @@
     </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="AI1:AJ1"/>
-    <mergeCell ref="E1:P1"/>
-    <mergeCell ref="Y1:AH1"/>
-    <mergeCell ref="E4:P4"/>
-    <mergeCell ref="Y4:AH4"/>
-    <mergeCell ref="AI4:AJ4"/>
     <mergeCell ref="B1:D1"/>
     <mergeCell ref="B4:D4"/>
     <mergeCell ref="Q1:X1"/>
@@ -34314,6 +34308,12 @@
     <mergeCell ref="V2:X2"/>
     <mergeCell ref="S4:U4"/>
     <mergeCell ref="V4:X4"/>
+    <mergeCell ref="AI1:AJ1"/>
+    <mergeCell ref="E1:P1"/>
+    <mergeCell ref="Y1:AH1"/>
+    <mergeCell ref="E4:P4"/>
+    <mergeCell ref="Y4:AH4"/>
+    <mergeCell ref="AI4:AJ4"/>
   </mergeCells>
   <conditionalFormatting sqref="S22:S37">
     <cfRule type="cellIs" dxfId="1" priority="1" operator="lessThan">
@@ -34331,13 +34331,13 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
-  <dimension ref="A1:AT52"/>
+  <dimension ref="A1:AX52"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="1" ySplit="5" topLeftCell="P6" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane xSplit="1" ySplit="5" topLeftCell="B6" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
-      <selection pane="bottomRight" activeCell="AN25" sqref="AN25"/>
+      <selection pane="bottomRight" activeCell="F34" sqref="F34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -34345,64 +34345,68 @@
     <col min="16" max="16" width="7.85546875" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="12.140625" bestFit="1" customWidth="1"/>
     <col min="18" max="20" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="21" max="27" width="11.7109375" customWidth="1"/>
-    <col min="28" max="28" width="12.5703125" customWidth="1"/>
-    <col min="40" max="40" width="14.5703125" customWidth="1"/>
+    <col min="21" max="29" width="11.7109375" customWidth="1"/>
+    <col min="30" max="32" width="12.5703125" customWidth="1"/>
+    <col min="44" max="44" width="14.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:46" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:50" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="38"/>
-      <c r="B1" s="258" t="s">
+      <c r="B1" s="257" t="s">
         <v>55</v>
       </c>
-      <c r="C1" s="258"/>
-      <c r="D1" s="258"/>
-      <c r="E1" s="258"/>
-      <c r="F1" s="258"/>
-      <c r="G1" s="258"/>
-      <c r="H1" s="258"/>
-      <c r="I1" s="258"/>
-      <c r="J1" s="258"/>
-      <c r="K1" s="258" t="s">
+      <c r="C1" s="257"/>
+      <c r="D1" s="257"/>
+      <c r="E1" s="257"/>
+      <c r="F1" s="257"/>
+      <c r="G1" s="257"/>
+      <c r="H1" s="257"/>
+      <c r="I1" s="257"/>
+      <c r="J1" s="257"/>
+      <c r="K1" s="257" t="s">
         <v>0</v>
       </c>
-      <c r="L1" s="258"/>
-      <c r="M1" s="258"/>
-      <c r="N1" s="258"/>
-      <c r="O1" s="258"/>
-      <c r="P1" s="258"/>
-      <c r="Q1" s="258"/>
-      <c r="R1" s="258"/>
-      <c r="S1" s="258"/>
-      <c r="T1" s="258"/>
-      <c r="U1" s="242" t="s">
+      <c r="L1" s="257"/>
+      <c r="M1" s="257"/>
+      <c r="N1" s="257"/>
+      <c r="O1" s="257"/>
+      <c r="P1" s="257"/>
+      <c r="Q1" s="257"/>
+      <c r="R1" s="257"/>
+      <c r="S1" s="257"/>
+      <c r="T1" s="257"/>
+      <c r="U1" s="241" t="s">
         <v>60</v>
       </c>
-      <c r="V1" s="240"/>
-      <c r="W1" s="240"/>
-      <c r="X1" s="240"/>
-      <c r="Y1" s="240"/>
-      <c r="Z1" s="240"/>
-      <c r="AA1" s="240"/>
-      <c r="AB1" s="240"/>
-      <c r="AC1" s="243" t="s">
+      <c r="V1" s="239"/>
+      <c r="W1" s="239"/>
+      <c r="X1" s="239"/>
+      <c r="Y1" s="239"/>
+      <c r="Z1" s="239"/>
+      <c r="AA1" s="239"/>
+      <c r="AB1" s="239"/>
+      <c r="AC1" s="239"/>
+      <c r="AD1" s="239"/>
+      <c r="AE1" s="239"/>
+      <c r="AF1" s="240"/>
+      <c r="AG1" s="242" t="s">
         <v>89</v>
       </c>
-      <c r="AD1" s="244"/>
-      <c r="AE1" s="244"/>
-      <c r="AF1" s="244"/>
-      <c r="AG1" s="244"/>
-      <c r="AH1" s="244"/>
-      <c r="AI1" s="244"/>
-      <c r="AJ1" s="244"/>
-      <c r="AK1" s="244"/>
-      <c r="AL1" s="245"/>
-      <c r="AM1" s="233" t="s">
+      <c r="AH1" s="243"/>
+      <c r="AI1" s="243"/>
+      <c r="AJ1" s="243"/>
+      <c r="AK1" s="243"/>
+      <c r="AL1" s="243"/>
+      <c r="AM1" s="243"/>
+      <c r="AN1" s="243"/>
+      <c r="AO1" s="243"/>
+      <c r="AP1" s="244"/>
+      <c r="AQ1" s="232" t="s">
         <v>92</v>
       </c>
-      <c r="AN1" s="234"/>
+      <c r="AR1" s="233"/>
     </row>
-    <row r="2" spans="1:46" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:50" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="10" t="s">
         <v>1</v>
       </c>
@@ -34469,54 +34473,58 @@
       <c r="V2" s="83" t="s">
         <v>57</v>
       </c>
-      <c r="W2" s="248" t="s">
+      <c r="W2" s="247" t="s">
         <v>58</v>
       </c>
-      <c r="X2" s="249"/>
-      <c r="Y2" s="249"/>
-      <c r="Z2" s="249" t="s">
+      <c r="X2" s="248"/>
+      <c r="Y2" s="248"/>
+      <c r="Z2" s="248"/>
+      <c r="AA2" s="250"/>
+      <c r="AB2" s="247" t="s">
         <v>59</v>
       </c>
-      <c r="AA2" s="249"/>
-      <c r="AB2" s="251"/>
-      <c r="AC2" s="3" t="s">
+      <c r="AC2" s="248"/>
+      <c r="AD2" s="248"/>
+      <c r="AE2" s="248"/>
+      <c r="AF2" s="250"/>
+      <c r="AG2" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="AD2" s="3" t="s">
+      <c r="AH2" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="AE2" s="3" t="s">
+      <c r="AI2" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="AF2" s="3" t="s">
+      <c r="AJ2" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="AG2" s="3" t="s">
+      <c r="AK2" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="AH2" s="3" t="s">
+      <c r="AL2" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="AI2" s="3" t="s">
+      <c r="AM2" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="AJ2" s="3" t="s">
+      <c r="AN2" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="AK2" s="19" t="s">
+      <c r="AO2" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="AL2" s="5" t="s">
+      <c r="AP2" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="AM2" s="11" t="s">
+      <c r="AQ2" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="AN2" s="5" t="s">
+      <c r="AR2" s="5" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="3" spans="1:46" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:50" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="10"/>
       <c r="B3" s="11"/>
       <c r="C3" s="3"/>
@@ -34553,88 +34561,104 @@
         <v>87</v>
       </c>
       <c r="Z3" s="84" t="s">
+        <v>6</v>
+      </c>
+      <c r="AA3" s="85" t="s">
+        <v>62</v>
+      </c>
+      <c r="AB3" s="84" t="s">
         <v>4</v>
       </c>
-      <c r="AA3" s="84" t="s">
+      <c r="AC3" s="84" t="s">
         <v>5</v>
       </c>
-      <c r="AB3" s="228" t="s">
+      <c r="AD3" s="268" t="s">
         <v>87</v>
       </c>
-      <c r="AC3" s="3"/>
-      <c r="AD3" s="3"/>
-      <c r="AE3" s="3"/>
-      <c r="AF3" s="3"/>
+      <c r="AE3" s="84" t="s">
+        <v>6</v>
+      </c>
+      <c r="AF3" s="85" t="s">
+        <v>62</v>
+      </c>
       <c r="AG3" s="3"/>
       <c r="AH3" s="3"/>
       <c r="AI3" s="3"/>
       <c r="AJ3" s="3"/>
-      <c r="AK3" s="19"/>
-      <c r="AL3" s="5"/>
-      <c r="AM3" s="203"/>
-      <c r="AN3" s="224"/>
+      <c r="AK3" s="3"/>
+      <c r="AL3" s="3"/>
+      <c r="AM3" s="3"/>
+      <c r="AN3" s="3"/>
+      <c r="AO3" s="19"/>
+      <c r="AP3" s="5"/>
+      <c r="AQ3" s="203"/>
+      <c r="AR3" s="224"/>
     </row>
-    <row r="4" spans="1:46" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:50" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="B4" s="252" t="s">
+      <c r="B4" s="251" t="s">
         <v>8</v>
       </c>
-      <c r="C4" s="239"/>
-      <c r="D4" s="239"/>
-      <c r="E4" s="239"/>
-      <c r="F4" s="239"/>
-      <c r="G4" s="239"/>
-      <c r="H4" s="239"/>
-      <c r="I4" s="239"/>
-      <c r="J4" s="260"/>
-      <c r="K4" s="239" t="s">
+      <c r="C4" s="238"/>
+      <c r="D4" s="238"/>
+      <c r="E4" s="238"/>
+      <c r="F4" s="238"/>
+      <c r="G4" s="238"/>
+      <c r="H4" s="238"/>
+      <c r="I4" s="238"/>
+      <c r="J4" s="259"/>
+      <c r="K4" s="238" t="s">
         <v>8</v>
       </c>
-      <c r="L4" s="239"/>
-      <c r="M4" s="239"/>
-      <c r="N4" s="239"/>
-      <c r="O4" s="239"/>
-      <c r="P4" s="239"/>
-      <c r="Q4" s="239"/>
-      <c r="R4" s="239"/>
-      <c r="S4" s="239"/>
-      <c r="T4" s="239"/>
+      <c r="L4" s="238"/>
+      <c r="M4" s="238"/>
+      <c r="N4" s="238"/>
+      <c r="O4" s="238"/>
+      <c r="P4" s="238"/>
+      <c r="Q4" s="238"/>
+      <c r="R4" s="238"/>
+      <c r="S4" s="238"/>
+      <c r="T4" s="238"/>
       <c r="U4" s="82" t="s">
         <v>9</v>
       </c>
       <c r="V4" s="82" t="s">
         <v>9</v>
       </c>
-      <c r="W4" s="252" t="s">
+      <c r="W4" s="251" t="s">
         <v>9</v>
       </c>
-      <c r="X4" s="239"/>
-      <c r="Y4" s="239"/>
-      <c r="Z4" s="252" t="s">
+      <c r="X4" s="238"/>
+      <c r="Y4" s="238"/>
+      <c r="Z4" s="79"/>
+      <c r="AA4" s="79"/>
+      <c r="AB4" s="251" t="s">
         <v>9</v>
       </c>
-      <c r="AA4" s="239"/>
-      <c r="AB4" s="239"/>
-      <c r="AC4" s="247" t="s">
+      <c r="AC4" s="238"/>
+      <c r="AD4" s="238"/>
+      <c r="AE4" s="79"/>
+      <c r="AF4" s="79"/>
+      <c r="AG4" s="246" t="s">
         <v>8</v>
       </c>
-      <c r="AD4" s="247"/>
-      <c r="AE4" s="247"/>
-      <c r="AF4" s="247"/>
-      <c r="AG4" s="247"/>
-      <c r="AH4" s="247"/>
-      <c r="AI4" s="247"/>
-      <c r="AJ4" s="247"/>
-      <c r="AK4" s="247"/>
-      <c r="AL4" s="247"/>
-      <c r="AM4" s="253" t="s">
+      <c r="AH4" s="246"/>
+      <c r="AI4" s="246"/>
+      <c r="AJ4" s="246"/>
+      <c r="AK4" s="246"/>
+      <c r="AL4" s="246"/>
+      <c r="AM4" s="246"/>
+      <c r="AN4" s="246"/>
+      <c r="AO4" s="246"/>
+      <c r="AP4" s="246"/>
+      <c r="AQ4" s="252" t="s">
         <v>8</v>
       </c>
-      <c r="AN4" s="254"/>
+      <c r="AR4" s="253"/>
     </row>
-    <row r="5" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A5" s="44" t="s">
         <v>10</v>
       </c>
@@ -34694,10 +34718,10 @@
         <f>Q5-R5-S5</f>
         <v>436.31667361835235</v>
       </c>
-      <c r="U5" s="230">
+      <c r="U5" s="229">
         <v>1.7158184937247267</v>
       </c>
-      <c r="V5" s="230">
+      <c r="V5" s="229">
         <f>U5</f>
         <v>1.7158184937247267</v>
       </c>
@@ -34710,70 +34734,82 @@
       <c r="Y5" s="111">
         <v>1.0824387039803123</v>
       </c>
-      <c r="Z5" s="187">
+      <c r="Z5" s="111">
+        <v>0.34283131369783426</v>
+      </c>
+      <c r="AA5" s="178">
+        <v>1.4792858651204461</v>
+      </c>
+      <c r="AB5" s="187">
         <v>1.1220004789136599</v>
       </c>
-      <c r="AA5" s="111">
+      <c r="AC5" s="111">
         <v>2.4131389662963039</v>
       </c>
-      <c r="AB5" s="111">
+      <c r="AD5" s="111">
         <v>1.0824387039803123</v>
       </c>
-      <c r="AC5" s="72">
-        <f>K5*$Z5</f>
+      <c r="AE5" s="111">
+        <v>2.1152391169621825</v>
+      </c>
+      <c r="AF5" s="178">
+        <v>1.4792858651204461</v>
+      </c>
+      <c r="AG5" s="72">
+        <f t="shared" ref="AG5:AG20" si="0">K5*$AB5</f>
         <v>9.0478118619597545</v>
       </c>
-      <c r="AD5" s="29">
-        <f>L5*$Z5</f>
+      <c r="AH5" s="29">
+        <f t="shared" ref="AH5:AH20" si="1">L5*$AB5</f>
         <v>86.584776957767147</v>
       </c>
-      <c r="AE5" s="29">
-        <f>M5*$Z5</f>
+      <c r="AI5" s="29">
+        <f t="shared" ref="AI5:AI20" si="2">M5*$AB5</f>
         <v>281.18902802246799</v>
       </c>
-      <c r="AF5" s="29">
-        <f>N5*$Z5</f>
+      <c r="AJ5" s="29">
+        <f t="shared" ref="AJ5:AJ20" si="3">N5*$AB5</f>
         <v>154.40129090450606</v>
       </c>
-      <c r="AG5" s="29">
-        <f>O5*$Z5</f>
+      <c r="AK5" s="29">
+        <f t="shared" ref="AK5:AK20" si="4">O5*$AB5</f>
         <v>11.466092253300445</v>
       </c>
-      <c r="AH5" s="29">
-        <f>P5*$Z5</f>
+      <c r="AL5" s="29">
+        <f t="shared" ref="AL5:AL20" si="5">P5*$AB5</f>
         <v>232.58100000000056</v>
       </c>
-      <c r="AI5" s="29">
-        <f>AJ5+AK5+AL5</f>
+      <c r="AM5" s="29">
+        <f>AN5+AO5+AP5</f>
         <v>775.27000000000191</v>
       </c>
-      <c r="AJ5" s="29">
-        <f>R5*$Z5</f>
+      <c r="AN5" s="29">
+        <f t="shared" ref="AN5:AN20" si="6">R5*$AB5</f>
         <v>23.048604071872024</v>
       </c>
-      <c r="AK5" s="29">
-        <f>S5*$Z5</f>
+      <c r="AO5" s="29">
+        <f t="shared" ref="AO5:AO20" si="7">S5*$AB5</f>
         <v>262.67387917032346</v>
       </c>
-      <c r="AL5" s="30">
-        <f>T5*$Z5</f>
+      <c r="AP5" s="30">
+        <f t="shared" ref="AP5:AP20" si="8">T5*$AB5</f>
         <v>489.54751675780642</v>
       </c>
-      <c r="AM5" s="72">
-        <f>R5*AA5</f>
+      <c r="AQ5" s="72">
+        <f t="shared" ref="AQ5:AQ20" si="9">R5*AC5</f>
         <v>49.571712000000005</v>
       </c>
-      <c r="AN5" s="216">
-        <f>(S5+T5)*AB5</f>
+      <c r="AR5" s="216">
+        <f t="shared" ref="AR5:AR20" si="10">(S5+T5)*AD5</f>
         <v>725.69804399999998</v>
       </c>
-      <c r="AO5" s="8"/>
-      <c r="AP5" s="8"/>
-      <c r="AR5" s="8"/>
       <c r="AS5" s="8"/>
       <c r="AT5" s="8"/>
+      <c r="AV5" s="8"/>
+      <c r="AW5" s="8"/>
+      <c r="AX5" s="8"/>
     </row>
-    <row r="6" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>11</v>
       </c>
@@ -34816,7 +34852,7 @@
         <v>0</v>
       </c>
       <c r="P6" s="39">
-        <f t="shared" ref="P6:P20" si="0">30/70*SUM(K6:O6)</f>
+        <f t="shared" ref="P6:P20" si="11">30/70*SUM(K6:O6)</f>
         <v>52.857798896274922</v>
       </c>
       <c r="Q6" s="39">
@@ -34833,11 +34869,11 @@
         <f>Q6-R6-S6</f>
         <v>97.818508571428566</v>
       </c>
-      <c r="U6" s="231">
+      <c r="U6" s="230">
         <v>2.8807897997459211</v>
       </c>
-      <c r="V6" s="231">
-        <f t="shared" ref="V6:V20" si="1">U6</f>
+      <c r="V6" s="230">
+        <f t="shared" ref="V6:V20" si="12">U6</f>
         <v>2.8807897997459211</v>
       </c>
       <c r="W6" s="185">
@@ -34849,70 +34885,82 @@
       <c r="Y6" s="180">
         <v>1.5606619455315904</v>
       </c>
-      <c r="Z6" s="188">
+      <c r="Z6" s="180">
+        <v>0.99931748632068484</v>
+      </c>
+      <c r="AA6" s="181">
+        <v>1.9919918514982764</v>
+      </c>
+      <c r="AB6" s="188">
         <v>1.6206123181197565</v>
       </c>
-      <c r="AA6" s="180">
+      <c r="AC6" s="180">
         <v>4.849480179027359</v>
       </c>
-      <c r="AB6" s="180">
+      <c r="AD6" s="180">
         <v>1.5606619455315904</v>
       </c>
-      <c r="AC6" s="70">
-        <f>K6*$Z6</f>
+      <c r="AE6" s="180">
+        <v>0.99931748632068484</v>
+      </c>
+      <c r="AF6" s="181">
+        <v>1.9919918514982764</v>
+      </c>
+      <c r="AG6" s="70">
+        <f t="shared" si="0"/>
         <v>0.68497463280090576</v>
       </c>
-      <c r="AD6" s="8">
-        <f>L6*$Z6</f>
+      <c r="AH6" s="8">
+        <f t="shared" si="1"/>
         <v>80.031022228171565</v>
       </c>
-      <c r="AE6" s="8">
-        <f>M6*$Z6</f>
+      <c r="AI6" s="8">
+        <f t="shared" si="2"/>
         <v>74.82367072758916</v>
       </c>
-      <c r="AF6" s="8">
-        <f>N6*$Z6</f>
+      <c r="AJ6" s="8">
+        <f t="shared" si="3"/>
         <v>44.338332411438422</v>
       </c>
-      <c r="AG6" s="8">
-        <f>O6*$Z6</f>
+      <c r="AK6" s="8">
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="AH6" s="8">
-        <f>P6*$Z6</f>
+      <c r="AL6" s="8">
+        <f t="shared" si="5"/>
         <v>85.662000000000006</v>
       </c>
-      <c r="AI6" s="8">
-        <f t="shared" ref="AI6:AI20" si="2">AJ6+AK6+AL6</f>
+      <c r="AM6" s="8">
+        <f t="shared" ref="AM6:AM20" si="13">AN6+AO6+AP6</f>
         <v>285.54000000000002</v>
       </c>
-      <c r="AJ6" s="8">
-        <f>R6*$Z6</f>
+      <c r="AN6" s="8">
+        <f t="shared" si="6"/>
         <v>5.2048605993264543</v>
       </c>
-      <c r="AK6" s="8">
-        <f>S6*$Z6</f>
+      <c r="AO6" s="8">
+        <f t="shared" si="7"/>
         <v>121.80925946971347</v>
       </c>
-      <c r="AL6" s="18">
-        <f>T6*$Z6</f>
+      <c r="AP6" s="18">
+        <f t="shared" si="8"/>
         <v>158.52587993096012</v>
       </c>
-      <c r="AM6" s="70">
-        <f>R6*AA6</f>
+      <c r="AQ6" s="70">
+        <f t="shared" si="9"/>
         <v>15.574895999999987</v>
       </c>
-      <c r="AN6" s="217">
-        <f>(S6+T6)*AB6</f>
+      <c r="AR6" s="217">
+        <f t="shared" si="10"/>
         <v>269.96486400000003</v>
       </c>
-      <c r="AO6" s="8"/>
-      <c r="AP6" s="8"/>
-      <c r="AR6" s="8"/>
       <c r="AS6" s="8"/>
       <c r="AT6" s="8"/>
+      <c r="AV6" s="8"/>
+      <c r="AW6" s="8"/>
+      <c r="AX6" s="8"/>
     </row>
-    <row r="7" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>12</v>
       </c>
@@ -34955,11 +35003,11 @@
         <v>0</v>
       </c>
       <c r="P7" s="39">
-        <f t="shared" si="0"/>
+        <f t="shared" si="11"/>
         <v>223.14866133713787</v>
       </c>
       <c r="Q7" s="39">
-        <f t="shared" ref="Q7:Q20" si="3">SUM(K7:P7)</f>
+        <f t="shared" ref="Q7:Q20" si="14">SUM(K7:P7)</f>
         <v>743.82887112379285</v>
       </c>
       <c r="R7" s="180">
@@ -34969,14 +35017,14 @@
         <v>192.49333785714285</v>
       </c>
       <c r="T7" s="181">
-        <f t="shared" ref="T7:T20" si="4">Q7-R7-S7</f>
+        <f t="shared" ref="T7:T20" si="15">Q7-R7-S7</f>
         <v>531.3947750000001</v>
       </c>
-      <c r="U7" s="231">
+      <c r="U7" s="230">
         <v>1.4750787020019531</v>
       </c>
-      <c r="V7" s="231">
-        <f t="shared" si="1"/>
+      <c r="V7" s="230">
+        <f t="shared" si="12"/>
         <v>1.4750787020019531</v>
       </c>
       <c r="W7" s="185">
@@ -34988,70 +35036,82 @@
       <c r="Y7" s="180">
         <v>1.0576195884447248</v>
       </c>
-      <c r="Z7" s="188">
+      <c r="Z7" s="180">
+        <v>0.91264523726207036</v>
+      </c>
+      <c r="AA7" s="181">
+        <v>1.1101353414700021</v>
+      </c>
+      <c r="AB7" s="188">
         <v>1.1305288523279819</v>
       </c>
-      <c r="AA7" s="180">
+      <c r="AC7" s="180">
         <v>3.7772150383052558</v>
       </c>
-      <c r="AB7" s="180">
+      <c r="AD7" s="180">
         <v>1.0576195884447248</v>
       </c>
-      <c r="AC7" s="70">
-        <f>K7*$Z7</f>
+      <c r="AE7" s="180">
+        <v>2.1152391169621825</v>
+      </c>
+      <c r="AF7" s="181">
+        <v>1.1101353414700021</v>
+      </c>
+      <c r="AG7" s="70">
+        <f t="shared" si="0"/>
         <v>6.3797289549468479</v>
       </c>
-      <c r="AD7" s="8">
-        <f>L7*$Z7</f>
+      <c r="AH7" s="8">
+        <f t="shared" si="1"/>
         <v>34.893207762677001</v>
-      </c>
-      <c r="AE7" s="8">
-        <f>M7*$Z7</f>
-        <v>140.36284461271478</v>
-      </c>
-      <c r="AF7" s="8">
-        <f>N7*$Z7</f>
-        <v>407.00821866966129</v>
-      </c>
-      <c r="AG7" s="8">
-        <f>O7*$Z7</f>
-        <v>0</v>
-      </c>
-      <c r="AH7" s="8">
-        <f>P7*$Z7</f>
-        <v>252.27599999999998</v>
       </c>
       <c r="AI7" s="8">
         <f t="shared" si="2"/>
+        <v>140.36284461271478</v>
+      </c>
+      <c r="AJ7" s="8">
+        <f t="shared" si="3"/>
+        <v>407.00821866966129</v>
+      </c>
+      <c r="AK7" s="8">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="AL7" s="8">
+        <f t="shared" si="5"/>
+        <v>252.27599999999998</v>
+      </c>
+      <c r="AM7" s="8">
+        <f t="shared" si="13"/>
         <v>840.92</v>
       </c>
-      <c r="AJ7" s="8">
-        <f>R7*$Z7</f>
+      <c r="AN7" s="8">
+        <f t="shared" si="6"/>
         <v>22.543602557745476</v>
       </c>
-      <c r="AK7" s="8">
-        <f>S7*$Z7</f>
+      <c r="AO7" s="8">
+        <f t="shared" si="7"/>
         <v>217.61927232841819</v>
       </c>
-      <c r="AL7" s="18">
-        <f>T7*$Z7</f>
+      <c r="AP7" s="18">
+        <f t="shared" si="8"/>
         <v>600.75712511383631</v>
       </c>
-      <c r="AM7" s="70">
-        <f>R7*AA7</f>
+      <c r="AQ7" s="70">
+        <f t="shared" si="9"/>
         <v>75.320532</v>
       </c>
-      <c r="AN7" s="217">
-        <f>(S7+T7)*AB7</f>
+      <c r="AR7" s="217">
+        <f t="shared" si="10"/>
         <v>765.59824800000001</v>
       </c>
-      <c r="AO7" s="8"/>
-      <c r="AP7" s="8"/>
-      <c r="AR7" s="8"/>
       <c r="AS7" s="8"/>
       <c r="AT7" s="8"/>
+      <c r="AV7" s="8"/>
+      <c r="AW7" s="8"/>
+      <c r="AX7" s="8"/>
     </row>
-    <row r="8" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>13</v>
       </c>
@@ -35094,11 +35154,11 @@
         <v>2045.5281</v>
       </c>
       <c r="P8" s="39">
-        <f t="shared" si="0"/>
+        <f t="shared" si="11"/>
         <v>3470.9181053571419</v>
       </c>
       <c r="Q8" s="39">
-        <f t="shared" si="3"/>
+        <f t="shared" si="14"/>
         <v>11569.727017857142</v>
       </c>
       <c r="R8" s="180">
@@ -35108,14 +35168,14 @@
         <v>3257.8222550892851</v>
       </c>
       <c r="T8" s="181">
-        <f t="shared" si="4"/>
+        <f t="shared" si="15"/>
         <v>7632.6547741964287</v>
       </c>
-      <c r="U8" s="231">
+      <c r="U8" s="230">
         <v>1.4685391547397617</v>
       </c>
-      <c r="V8" s="231">
-        <f t="shared" si="1"/>
+      <c r="V8" s="230">
+        <f t="shared" si="12"/>
         <v>1.4685391547397617</v>
       </c>
       <c r="W8" s="185">
@@ -35127,70 +35187,82 @@
       <c r="Y8" s="180">
         <v>0.91153292709815303</v>
       </c>
-      <c r="Z8" s="188">
+      <c r="Z8" s="180">
+        <v>1.9713861264122234</v>
+      </c>
+      <c r="AA8" s="181">
+        <v>0.45915908837485314</v>
+      </c>
+      <c r="AB8" s="188">
         <v>1.056757863096452</v>
       </c>
-      <c r="AA8" s="180">
+      <c r="AC8" s="180">
         <v>3.3846356815333842</v>
       </c>
-      <c r="AB8" s="180">
+      <c r="AD8" s="180">
         <v>1.6496659822479089</v>
       </c>
-      <c r="AC8" s="70">
-        <f>K8*$Z8</f>
+      <c r="AE8" s="180">
+        <v>1.9713861264122234</v>
+      </c>
+      <c r="AF8" s="181">
+        <v>1.7375621622004116</v>
+      </c>
+      <c r="AG8" s="70">
+        <f t="shared" si="0"/>
         <v>258.77041145215441</v>
       </c>
-      <c r="AD8" s="8">
-        <f>L8*$Z8</f>
+      <c r="AH8" s="8">
+        <f t="shared" si="1"/>
         <v>1332.597569141745</v>
-      </c>
-      <c r="AE8" s="8">
-        <f>M8*$Z8</f>
-        <v>1498.1886598332553</v>
-      </c>
-      <c r="AF8" s="8">
-        <f>N8*$Z8</f>
-        <v>3307.2954557130997</v>
-      </c>
-      <c r="AG8" s="8">
-        <f>O8*$Z8</f>
-        <v>2161.6279038597459</v>
-      </c>
-      <c r="AH8" s="8">
-        <f>P8*$Z8</f>
-        <v>3667.9199999999992</v>
       </c>
       <c r="AI8" s="8">
         <f t="shared" si="2"/>
+        <v>1498.1886598332553</v>
+      </c>
+      <c r="AJ8" s="8">
+        <f t="shared" si="3"/>
+        <v>3307.2954557130997</v>
+      </c>
+      <c r="AK8" s="8">
+        <f t="shared" si="4"/>
+        <v>2161.6279038597459</v>
+      </c>
+      <c r="AL8" s="8">
+        <f t="shared" si="5"/>
+        <v>3667.9199999999992</v>
+      </c>
+      <c r="AM8" s="8">
+        <f t="shared" si="13"/>
         <v>12226.400000000001</v>
       </c>
-      <c r="AJ8" s="8">
-        <f>R8*$Z8</f>
+      <c r="AN8" s="8">
+        <f t="shared" si="6"/>
         <v>717.8027664310323</v>
       </c>
-      <c r="AK8" s="8">
-        <f>S8*$Z8</f>
+      <c r="AO8" s="8">
+        <f t="shared" si="7"/>
         <v>3442.7292846362175</v>
       </c>
-      <c r="AL8" s="18">
-        <f>T8*$Z8</f>
+      <c r="AP8" s="18">
+        <f t="shared" si="8"/>
         <v>8065.8679489327506</v>
       </c>
-      <c r="AM8" s="70">
-        <f>R8*AA8</f>
+      <c r="AQ8" s="70">
+        <f t="shared" si="9"/>
         <v>2299.0137480000003</v>
       </c>
-      <c r="AN8" s="217">
-        <f>(S8+T8)*AB8</f>
+      <c r="AR8" s="217">
+        <f t="shared" si="10"/>
         <v>17965.649485664908</v>
       </c>
-      <c r="AO8" s="8"/>
-      <c r="AP8" s="8"/>
-      <c r="AR8" s="8"/>
       <c r="AS8" s="8"/>
       <c r="AT8" s="8"/>
+      <c r="AV8" s="8"/>
+      <c r="AW8" s="8"/>
+      <c r="AX8" s="8"/>
     </row>
-    <row r="9" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>14</v>
       </c>
@@ -35233,11 +35305,11 @@
         <v>53.725890875912398</v>
       </c>
       <c r="P9" s="39">
-        <f t="shared" si="0"/>
+        <f t="shared" si="11"/>
         <v>273.14333180396244</v>
       </c>
       <c r="Q9" s="39">
-        <f t="shared" si="3"/>
+        <f t="shared" si="14"/>
         <v>910.47777267987476</v>
       </c>
       <c r="R9" s="180">
@@ -35247,14 +35319,14 @@
         <v>331.62901986965585</v>
       </c>
       <c r="T9" s="181">
-        <f t="shared" si="4"/>
+        <f t="shared" si="15"/>
         <v>534.60100092283619</v>
       </c>
-      <c r="U9" s="231">
+      <c r="U9" s="230">
         <v>2.3577406738360649</v>
       </c>
-      <c r="V9" s="231">
-        <f t="shared" si="1"/>
+      <c r="V9" s="230">
+        <f t="shared" si="12"/>
         <v>2.3577406738360649</v>
       </c>
       <c r="W9" s="185">
@@ -35266,68 +35338,80 @@
       <c r="Y9" s="180">
         <v>1.4144822859856947</v>
       </c>
-      <c r="Z9" s="188">
+      <c r="Z9" s="180">
+        <v>1.094456969244296</v>
+      </c>
+      <c r="AA9" s="181">
+        <v>1.6130035793263797</v>
+      </c>
+      <c r="AB9" s="188">
         <v>1.5131725796500084</v>
       </c>
-      <c r="AA9" s="180">
+      <c r="AC9" s="180">
         <v>3.4451781502478749</v>
       </c>
-      <c r="AB9" s="180">
+      <c r="AD9" s="180">
         <v>1.4144822859856947</v>
       </c>
-      <c r="AC9" s="70">
-        <f>K9*$Z9</f>
+      <c r="AE9" s="180">
+        <v>1.094456969244296</v>
+      </c>
+      <c r="AF9" s="181">
+        <v>1.6130035793263797</v>
+      </c>
+      <c r="AG9" s="70">
+        <f t="shared" si="0"/>
         <v>31.486095037357373</v>
       </c>
-      <c r="AD9" s="8">
-        <f>L9*$Z9</f>
+      <c r="AH9" s="8">
+        <f t="shared" si="1"/>
         <v>364.28585765993995</v>
-      </c>
-      <c r="AE9" s="8">
-        <f>M9*$Z9</f>
-        <v>80.060750651218228</v>
-      </c>
-      <c r="AF9" s="8">
-        <f>N9*$Z9</f>
-        <v>407.26775176078542</v>
-      </c>
-      <c r="AG9" s="8">
-        <f>O9*$Z9</f>
-        <v>81.296544890699209</v>
-      </c>
-      <c r="AH9" s="8">
-        <f>P9*$Z9</f>
-        <v>413.31300000000005</v>
       </c>
       <c r="AI9" s="8">
         <f t="shared" si="2"/>
+        <v>80.060750651218228</v>
+      </c>
+      <c r="AJ9" s="8">
+        <f t="shared" si="3"/>
+        <v>407.26775176078542</v>
+      </c>
+      <c r="AK9" s="8">
+        <f t="shared" si="4"/>
+        <v>81.296544890699209</v>
+      </c>
+      <c r="AL9" s="8">
+        <f t="shared" si="5"/>
+        <v>413.31300000000005</v>
+      </c>
+      <c r="AM9" s="8">
+        <f t="shared" si="13"/>
         <v>1377.71</v>
       </c>
-      <c r="AJ9" s="8">
-        <f>R9*$Z9</f>
+      <c r="AN9" s="8">
+        <f t="shared" si="6"/>
         <v>66.954484867144387</v>
       </c>
-      <c r="AK9" s="8">
-        <f>S9*$Z9</f>
+      <c r="AO9" s="8">
+        <f t="shared" si="7"/>
         <v>501.81193948297101</v>
       </c>
-      <c r="AL9" s="18">
-        <f>T9*$Z9</f>
+      <c r="AP9" s="18">
+        <f t="shared" si="8"/>
         <v>808.94357564988456</v>
       </c>
-      <c r="AM9" s="70">
-        <f>R9*AA9</f>
+      <c r="AQ9" s="70">
+        <f t="shared" si="9"/>
         <v>152.44138800000002</v>
       </c>
-      <c r="AN9" s="217">
-        <f>(S9+T9)*AB9</f>
+      <c r="AR9" s="217">
+        <f t="shared" si="10"/>
         <v>1225.26702</v>
       </c>
-      <c r="AR9" s="8"/>
-      <c r="AS9" s="8"/>
-      <c r="AT9" s="8"/>
+      <c r="AV9" s="8"/>
+      <c r="AW9" s="8"/>
+      <c r="AX9" s="8"/>
     </row>
-    <row r="10" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>15</v>
       </c>
@@ -35370,11 +35454,11 @@
         <v>56.305527372262802</v>
       </c>
       <c r="P10" s="39">
-        <f t="shared" si="0"/>
+        <f t="shared" si="11"/>
         <v>132.71004480954119</v>
       </c>
       <c r="Q10" s="39">
-        <f t="shared" si="3"/>
+        <f t="shared" si="14"/>
         <v>442.36681603180398</v>
       </c>
       <c r="R10" s="180">
@@ -35384,14 +35468,14 @@
         <v>112.10674546246091</v>
       </c>
       <c r="T10" s="181">
-        <f t="shared" si="4"/>
+        <f t="shared" si="15"/>
         <v>313.66444151720543</v>
       </c>
-      <c r="U10" s="231">
+      <c r="U10" s="230">
         <v>2.4211502128146489</v>
       </c>
-      <c r="V10" s="231">
-        <f t="shared" si="1"/>
+      <c r="V10" s="230">
+        <f t="shared" si="12"/>
         <v>2.4211502128146489</v>
       </c>
       <c r="W10" s="185">
@@ -35403,68 +35487,80 @@
       <c r="Y10" s="180">
         <v>1.6785700438534636</v>
       </c>
-      <c r="Z10" s="188">
+      <c r="Z10" s="180">
+        <v>2.4719680413235743</v>
+      </c>
+      <c r="AA10" s="181">
+        <v>1.3950018238710629</v>
+      </c>
+      <c r="AB10" s="188">
         <v>1.8082052518661162</v>
       </c>
-      <c r="AA10" s="180">
+      <c r="AC10" s="180">
         <v>5.1339650779326984</v>
       </c>
-      <c r="AB10" s="180">
+      <c r="AD10" s="180">
         <v>1.6785700438534636</v>
       </c>
-      <c r="AC10" s="70">
-        <f>K10*$Z10</f>
+      <c r="AE10" s="180">
+        <v>2.4719680413235743</v>
+      </c>
+      <c r="AF10" s="181">
+        <v>1.3950018238710629</v>
+      </c>
+      <c r="AG10" s="70">
+        <f t="shared" si="0"/>
         <v>14.19079481664528</v>
       </c>
-      <c r="AD10" s="8">
-        <f>L10*$Z10</f>
+      <c r="AH10" s="8">
+        <f t="shared" si="1"/>
         <v>16.742805298866521</v>
-      </c>
-      <c r="AE10" s="8">
-        <f>M10*$Z10</f>
-        <v>222.91915986055855</v>
-      </c>
-      <c r="AF10" s="8">
-        <f>N10*$Z10</f>
-        <v>204.25828972031272</v>
-      </c>
-      <c r="AG10" s="8">
-        <f>O10*$Z10</f>
-        <v>101.81195030361697</v>
-      </c>
-      <c r="AH10" s="8">
-        <f>P10*$Z10</f>
-        <v>239.96699999999998</v>
       </c>
       <c r="AI10" s="8">
         <f t="shared" si="2"/>
+        <v>222.91915986055855</v>
+      </c>
+      <c r="AJ10" s="8">
+        <f t="shared" si="3"/>
+        <v>204.25828972031272</v>
+      </c>
+      <c r="AK10" s="8">
+        <f t="shared" si="4"/>
+        <v>101.81195030361697</v>
+      </c>
+      <c r="AL10" s="8">
+        <f t="shared" si="5"/>
+        <v>239.96699999999998</v>
+      </c>
+      <c r="AM10" s="8">
+        <f t="shared" si="13"/>
         <v>799.8900000000001</v>
       </c>
-      <c r="AJ10" s="8">
-        <f>R10*$Z10</f>
+      <c r="AN10" s="8">
+        <f t="shared" si="6"/>
         <v>30.008303610097187</v>
       </c>
-      <c r="AK10" s="8">
-        <f>S10*$Z10</f>
+      <c r="AO10" s="8">
+        <f t="shared" si="7"/>
         <v>202.71200591483972</v>
       </c>
-      <c r="AL10" s="18">
-        <f>T10*$Z10</f>
+      <c r="AP10" s="18">
+        <f t="shared" si="8"/>
         <v>567.16969047506313</v>
       </c>
-      <c r="AM10" s="70">
-        <f>R10*AA10</f>
+      <c r="AQ10" s="70">
+        <f t="shared" si="9"/>
         <v>85.20138</v>
       </c>
-      <c r="AN10" s="217">
-        <f>(S10+T10)*AB10</f>
+      <c r="AR10" s="217">
+        <f t="shared" si="10"/>
         <v>714.68675999999982</v>
       </c>
-      <c r="AR10" s="8"/>
-      <c r="AS10" s="8"/>
-      <c r="AT10" s="8"/>
+      <c r="AV10" s="8"/>
+      <c r="AW10" s="8"/>
+      <c r="AX10" s="8"/>
     </row>
-    <row r="11" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>16</v>
       </c>
@@ -35507,11 +35603,11 @@
         <v>83.983325912408702</v>
       </c>
       <c r="P11" s="39">
-        <f t="shared" si="0"/>
+        <f t="shared" si="11"/>
         <v>534.30895102988939</v>
       </c>
       <c r="Q11" s="39">
-        <f t="shared" si="3"/>
+        <f t="shared" si="14"/>
         <v>1781.0298367662981</v>
       </c>
       <c r="R11" s="180">
@@ -35521,14 +35617,14 @@
         <v>559.1503121444631</v>
       </c>
       <c r="T11" s="181">
-        <f t="shared" si="4"/>
+        <f t="shared" si="15"/>
         <v>1177.6277168505731</v>
       </c>
-      <c r="U11" s="231">
+      <c r="U11" s="230">
         <v>3.3364608108129992</v>
       </c>
-      <c r="V11" s="231">
-        <f t="shared" si="1"/>
+      <c r="V11" s="230">
+        <f t="shared" si="12"/>
         <v>3.3364608108129992</v>
       </c>
       <c r="W11" s="185">
@@ -35540,68 +35636,80 @@
       <c r="Y11" s="180">
         <v>2.1956630290898849</v>
       </c>
-      <c r="Z11" s="188">
+      <c r="Z11" s="180">
+        <v>1.8533777295509326</v>
+      </c>
+      <c r="AA11" s="181">
+        <v>2.3581837725651766</v>
+      </c>
+      <c r="AB11" s="188">
         <v>2.27075364854243</v>
       </c>
-      <c r="AA11" s="180">
+      <c r="AC11" s="180">
         <v>5.217911575353849</v>
       </c>
-      <c r="AB11" s="180">
+      <c r="AD11" s="180">
         <v>2.1956630290898849</v>
       </c>
-      <c r="AC11" s="70">
-        <f>K11*$Z11</f>
+      <c r="AE11" s="180">
+        <v>1.8533777295509326</v>
+      </c>
+      <c r="AF11" s="181">
+        <v>2.3581837725651766</v>
+      </c>
+      <c r="AG11" s="70">
+        <f t="shared" si="0"/>
         <v>34.660783691351654</v>
       </c>
-      <c r="AD11" s="8">
-        <f>L11*$Z11</f>
+      <c r="AH11" s="8">
+        <f t="shared" si="1"/>
         <v>301.36840673738271</v>
-      </c>
-      <c r="AE11" s="8">
-        <f>M11*$Z11</f>
-        <v>1471.9633711829838</v>
-      </c>
-      <c r="AF11" s="8">
-        <f>N11*$Z11</f>
-        <v>832.2979946559517</v>
-      </c>
-      <c r="AG11" s="8">
-        <f>O11*$Z11</f>
-        <v>190.70544373233005</v>
-      </c>
-      <c r="AH11" s="8">
-        <f>P11*$Z11</f>
-        <v>1213.2839999999999</v>
       </c>
       <c r="AI11" s="8">
         <f t="shared" si="2"/>
+        <v>1471.9633711829838</v>
+      </c>
+      <c r="AJ11" s="8">
+        <f t="shared" si="3"/>
+        <v>832.2979946559517</v>
+      </c>
+      <c r="AK11" s="8">
+        <f t="shared" si="4"/>
+        <v>190.70544373233005</v>
+      </c>
+      <c r="AL11" s="8">
+        <f t="shared" si="5"/>
+        <v>1213.2839999999999</v>
+      </c>
+      <c r="AM11" s="8">
+        <f t="shared" si="13"/>
         <v>4044.2799999999993</v>
       </c>
-      <c r="AJ11" s="8">
-        <f>R11*$Z11</f>
+      <c r="AN11" s="8">
+        <f t="shared" si="6"/>
         <v>100.48495395119085</v>
       </c>
-      <c r="AK11" s="8">
-        <f>S11*$Z11</f>
+      <c r="AO11" s="8">
+        <f t="shared" si="7"/>
         <v>1269.6926113856782</v>
       </c>
-      <c r="AL11" s="18">
-        <f>T11*$Z11</f>
+      <c r="AP11" s="18">
+        <f t="shared" si="8"/>
         <v>2674.1024346631302</v>
       </c>
-      <c r="AM11" s="70">
-        <f>R11*AA11</f>
+      <c r="AQ11" s="70">
+        <f t="shared" si="9"/>
         <v>230.90202000000002</v>
       </c>
-      <c r="AN11" s="217">
-        <f>(S11+T11)*AB11</f>
+      <c r="AR11" s="217">
+        <f t="shared" si="10"/>
         <v>3813.3793080000005</v>
       </c>
-      <c r="AR11" s="8"/>
-      <c r="AS11" s="8"/>
-      <c r="AT11" s="8"/>
+      <c r="AV11" s="8"/>
+      <c r="AW11" s="8"/>
+      <c r="AX11" s="8"/>
     </row>
-    <row r="12" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>17</v>
       </c>
@@ -35644,7 +35752,7 @@
         <v>135.485163</v>
       </c>
       <c r="P12" s="39">
-        <f t="shared" si="0"/>
+        <f t="shared" si="11"/>
         <v>317.09588957142859</v>
       </c>
       <c r="Q12" s="39">
@@ -35661,11 +35769,11 @@
         <f>Q12-R12-S12</f>
         <v>774.3631892857145</v>
       </c>
-      <c r="U12" s="231">
+      <c r="U12" s="230">
         <v>1.5912300685966148</v>
       </c>
-      <c r="V12" s="231">
-        <f t="shared" si="1"/>
+      <c r="V12" s="230">
+        <f t="shared" si="12"/>
         <v>1.5912300685966148</v>
       </c>
       <c r="W12" s="185">
@@ -35677,68 +35785,80 @@
       <c r="Y12" s="180">
         <v>1.1567724390655256</v>
       </c>
-      <c r="Z12" s="188">
+      <c r="Z12" s="180">
+        <v>1.8511389487990497</v>
+      </c>
+      <c r="AA12" s="181">
+        <v>0.95207729680442987</v>
+      </c>
+      <c r="AB12" s="188">
         <v>1.2797422273384271</v>
       </c>
-      <c r="AA12" s="180">
+      <c r="AC12" s="180">
         <v>3.548486924163698</v>
       </c>
-      <c r="AB12" s="180">
+      <c r="AD12" s="180">
         <v>1.1567724390655256</v>
       </c>
-      <c r="AC12" s="70">
-        <f>K12*$Z12</f>
+      <c r="AE12" s="180">
+        <v>1.8511389487990497</v>
+      </c>
+      <c r="AF12" s="181">
+        <v>1.7375621622004116</v>
+      </c>
+      <c r="AG12" s="70">
+        <f t="shared" si="0"/>
         <v>34.921605899611002</v>
       </c>
-      <c r="AD12" s="8">
-        <f>L12*$Z12</f>
+      <c r="AH12" s="8">
+        <f t="shared" si="1"/>
         <v>39.498603975686883</v>
       </c>
-      <c r="AE12" s="8">
-        <f>M12*$Z12</f>
+      <c r="AI12" s="8">
+        <f t="shared" si="2"/>
         <v>106.9762122676738</v>
       </c>
-      <c r="AF12" s="8">
-        <f>N12*$Z12</f>
+      <c r="AJ12" s="8">
+        <f t="shared" si="3"/>
         <v>592.08649358809828</v>
       </c>
-      <c r="AG12" s="8">
-        <f>O12*$Z12</f>
+      <c r="AK12" s="8">
+        <f t="shared" si="4"/>
         <v>173.38608426892986</v>
       </c>
-      <c r="AH12" s="8">
-        <f>P12*$Z12</f>
+      <c r="AL12" s="8">
+        <f t="shared" si="5"/>
         <v>405.80099999999993</v>
       </c>
-      <c r="AI12" s="8">
-        <f>AJ12+AK12+AL12</f>
+      <c r="AM12" s="8">
+        <f>AN12+AO12+AP12</f>
         <v>1352.67</v>
       </c>
-      <c r="AJ12" s="8">
-        <f>R12*$Z12</f>
+      <c r="AN12" s="8">
+        <f t="shared" si="6"/>
         <v>69.548127300751631</v>
       </c>
-      <c r="AK12" s="8">
-        <f>S12*$Z12</f>
+      <c r="AO12" s="8">
+        <f t="shared" si="7"/>
         <v>292.13660007386005</v>
       </c>
-      <c r="AL12" s="18">
-        <f>T12*$Z12</f>
+      <c r="AP12" s="18">
+        <f t="shared" si="8"/>
         <v>990.98527262538835</v>
       </c>
-      <c r="AM12" s="70">
-        <f>R12*AA12</f>
+      <c r="AQ12" s="70">
+        <f t="shared" si="9"/>
         <v>192.844008</v>
       </c>
-      <c r="AN12" s="217">
-        <f>(S12+T12)*AB12</f>
+      <c r="AR12" s="217">
+        <f t="shared" si="10"/>
         <v>1159.8273360000001</v>
       </c>
-      <c r="AR12" s="8"/>
-      <c r="AS12" s="8"/>
-      <c r="AT12" s="8"/>
+      <c r="AV12" s="8"/>
+      <c r="AW12" s="8"/>
+      <c r="AX12" s="8"/>
     </row>
-    <row r="13" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>18</v>
       </c>
@@ -35781,11 +35901,11 @@
         <v>261.58506240875897</v>
       </c>
       <c r="P13" s="39">
-        <f t="shared" si="0"/>
+        <f t="shared" si="11"/>
         <v>616.0372981751824</v>
       </c>
       <c r="Q13" s="39">
-        <f t="shared" si="3"/>
+        <f t="shared" si="14"/>
         <v>2053.4576605839416</v>
       </c>
       <c r="R13" s="180">
@@ -35795,14 +35915,14 @@
         <v>470.38377446298227</v>
       </c>
       <c r="T13" s="181">
-        <f t="shared" si="4"/>
+        <f t="shared" si="15"/>
         <v>1534.9056777163712</v>
       </c>
-      <c r="U13" s="231">
+      <c r="U13" s="230">
         <v>2.0519110354253987</v>
       </c>
-      <c r="V13" s="231">
-        <f t="shared" si="1"/>
+      <c r="V13" s="230">
+        <f t="shared" si="12"/>
         <v>2.0519110354253987</v>
       </c>
       <c r="W13" s="185">
@@ -35814,68 +35934,80 @@
       <c r="Y13" s="180">
         <v>0.84665546221012566</v>
       </c>
-      <c r="Z13" s="188">
+      <c r="Z13" s="180">
+        <v>0.64344007687241933</v>
+      </c>
+      <c r="AA13" s="181">
+        <v>0.9089323964685988</v>
+      </c>
+      <c r="AB13" s="188">
         <v>1.6145656785206102</v>
       </c>
-      <c r="AA13" s="180">
+      <c r="AC13" s="180">
         <v>1.396810847413442</v>
       </c>
-      <c r="AB13" s="180">
+      <c r="AD13" s="180">
         <v>1.6496659822479089</v>
       </c>
-      <c r="AC13" s="70">
-        <f>K13*$Z13</f>
+      <c r="AE13" s="180">
+        <v>2.1152391169621825</v>
+      </c>
+      <c r="AF13" s="181">
+        <v>1.7375621622004116</v>
+      </c>
+      <c r="AG13" s="70">
+        <f t="shared" si="0"/>
         <v>22.784750855282851</v>
       </c>
-      <c r="AD13" s="8">
-        <f>L13*$Z13</f>
+      <c r="AH13" s="8">
+        <f t="shared" si="1"/>
         <v>19.933104953879749</v>
-      </c>
-      <c r="AE13" s="8">
-        <f>M13*$Z13</f>
-        <v>622.51194301040641</v>
-      </c>
-      <c r="AF13" s="8">
-        <f>N13*$Z13</f>
-        <v>1233.2335201534161</v>
-      </c>
-      <c r="AG13" s="8">
-        <f>O13*$Z13</f>
-        <v>422.34626377885411</v>
-      </c>
-      <c r="AH13" s="8">
-        <f>P13*$Z13</f>
-        <v>994.63267832221686</v>
       </c>
       <c r="AI13" s="8">
         <f t="shared" si="2"/>
+        <v>622.51194301040641</v>
+      </c>
+      <c r="AJ13" s="8">
+        <f t="shared" si="3"/>
+        <v>1233.2335201534161</v>
+      </c>
+      <c r="AK13" s="8">
+        <f t="shared" si="4"/>
+        <v>422.34626377885411</v>
+      </c>
+      <c r="AL13" s="8">
+        <f t="shared" si="5"/>
+        <v>994.63267832221686</v>
+      </c>
+      <c r="AM13" s="8">
+        <f t="shared" si="13"/>
         <v>3315.4422610740567</v>
       </c>
-      <c r="AJ13" s="8">
-        <f>R13*$Z13</f>
+      <c r="AN13" s="8">
+        <f t="shared" si="6"/>
         <v>77.770736085875967</v>
       </c>
-      <c r="AK13" s="8">
-        <f>S13*$Z13</f>
+      <c r="AO13" s="8">
+        <f t="shared" si="7"/>
         <v>759.46549798091064</v>
       </c>
-      <c r="AL13" s="18">
-        <f>T13*$Z13</f>
+      <c r="AP13" s="18">
+        <f t="shared" si="8"/>
         <v>2478.2060270072698</v>
       </c>
-      <c r="AM13" s="70">
-        <f>R13*AA13</f>
+      <c r="AQ13" s="70">
+        <f t="shared" si="9"/>
         <v>67.281875999999997</v>
       </c>
-      <c r="AN13" s="217">
-        <f>(S13+T13)*AB13</f>
+      <c r="AR13" s="217">
+        <f t="shared" si="10"/>
         <v>3308.0577938208244</v>
       </c>
-      <c r="AR13" s="8"/>
-      <c r="AS13" s="8"/>
-      <c r="AT13" s="8"/>
+      <c r="AV13" s="8"/>
+      <c r="AW13" s="8"/>
+      <c r="AX13" s="8"/>
     </row>
-    <row r="14" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>19</v>
       </c>
@@ -35918,11 +36050,11 @@
         <v>198.495</v>
       </c>
       <c r="P14" s="39">
-        <f t="shared" si="0"/>
+        <f t="shared" si="11"/>
         <v>381.11930357142853</v>
       </c>
       <c r="Q14" s="39">
-        <f t="shared" si="3"/>
+        <f t="shared" si="14"/>
         <v>1270.3976785714285</v>
       </c>
       <c r="R14" s="180">
@@ -35932,14 +36064,14 @@
         <v>234.74837196428575</v>
       </c>
       <c r="T14" s="181">
-        <f t="shared" si="4"/>
+        <f t="shared" si="15"/>
         <v>968.12030660714277</v>
       </c>
-      <c r="U14" s="231">
+      <c r="U14" s="230">
         <v>1.882709580425066</v>
       </c>
-      <c r="V14" s="231">
-        <f t="shared" si="1"/>
+      <c r="V14" s="230">
+        <f t="shared" si="12"/>
         <v>1.882709580425066</v>
       </c>
       <c r="W14" s="185">
@@ -35951,68 +36083,80 @@
       <c r="Y14" s="180">
         <v>1.51089323080423</v>
       </c>
-      <c r="Z14" s="188">
+      <c r="Z14" s="180">
+        <v>2.5028230827917586</v>
+      </c>
+      <c r="AA14" s="181">
+        <v>1.2703715556904176</v>
+      </c>
+      <c r="AB14" s="188">
         <v>1.5864008837502654</v>
       </c>
-      <c r="AA14" s="180">
+      <c r="AC14" s="180">
         <v>2.9313614002872836</v>
       </c>
-      <c r="AB14" s="180">
+      <c r="AD14" s="180">
         <v>1.51089323080423</v>
       </c>
-      <c r="AC14" s="70">
-        <f>K14*$Z14</f>
+      <c r="AE14" s="180">
+        <v>2.5028230827917586</v>
+      </c>
+      <c r="AF14" s="181">
+        <v>1.2703715556904176</v>
+      </c>
+      <c r="AG14" s="70">
+        <f t="shared" si="0"/>
         <v>54.026468496999037</v>
       </c>
-      <c r="AD14" s="8">
-        <f>L14*$Z14</f>
+      <c r="AH14" s="8">
+        <f t="shared" si="1"/>
         <v>7.3445205114765102</v>
-      </c>
-      <c r="AE14" s="8">
-        <f>M14*$Z14</f>
-        <v>34.591788550351282</v>
-      </c>
-      <c r="AF14" s="8">
-        <f>N14*$Z14</f>
-        <v>999.89657902116426</v>
-      </c>
-      <c r="AG14" s="8">
-        <f>O14*$Z14</f>
-        <v>314.89264342000894</v>
-      </c>
-      <c r="AH14" s="8">
-        <f>P14*$Z14</f>
-        <v>604.60799999999995</v>
       </c>
       <c r="AI14" s="8">
         <f t="shared" si="2"/>
+        <v>34.591788550351282</v>
+      </c>
+      <c r="AJ14" s="8">
+        <f t="shared" si="3"/>
+        <v>999.89657902116426</v>
+      </c>
+      <c r="AK14" s="8">
+        <f t="shared" si="4"/>
+        <v>314.89264342000894</v>
+      </c>
+      <c r="AL14" s="8">
+        <f t="shared" si="5"/>
+        <v>604.60799999999995</v>
+      </c>
+      <c r="AM14" s="8">
+        <f t="shared" si="13"/>
         <v>2015.3599999999997</v>
       </c>
-      <c r="AJ14" s="8">
-        <f>R14*$Z14</f>
+      <c r="AN14" s="8">
+        <f t="shared" si="6"/>
         <v>107.12806527877169</v>
       </c>
-      <c r="AK14" s="8">
-        <f>S14*$Z14</f>
+      <c r="AO14" s="8">
+        <f t="shared" si="7"/>
         <v>372.40502474307897</v>
       </c>
-      <c r="AL14" s="18">
-        <f>T14*$Z14</f>
+      <c r="AP14" s="18">
+        <f t="shared" si="8"/>
         <v>1535.8269099781492</v>
       </c>
-      <c r="AM14" s="70">
-        <f>R14*AA14</f>
+      <c r="AQ14" s="70">
+        <f t="shared" si="9"/>
         <v>197.95190400000001</v>
       </c>
-      <c r="AN14" s="217">
-        <f>(S14+T14)*AB14</f>
+      <c r="AR14" s="217">
+        <f t="shared" si="10"/>
         <v>1817.4061440000005</v>
       </c>
-      <c r="AR14" s="8"/>
-      <c r="AS14" s="8"/>
-      <c r="AT14" s="8"/>
+      <c r="AV14" s="8"/>
+      <c r="AW14" s="8"/>
+      <c r="AX14" s="8"/>
     </row>
-    <row r="15" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>20</v>
       </c>
@@ -36055,11 +36199,11 @@
         <v>62.2585346715329</v>
       </c>
       <c r="P15" s="39">
-        <f t="shared" si="0"/>
+        <f t="shared" si="11"/>
         <v>755.37014343065698</v>
       </c>
       <c r="Q15" s="39">
-        <f t="shared" si="3"/>
+        <f t="shared" si="14"/>
         <v>2517.9004781021899</v>
       </c>
       <c r="R15" s="180">
@@ -36069,14 +36213,14 @@
         <v>864.41588335245046</v>
       </c>
       <c r="T15" s="181">
-        <f t="shared" si="4"/>
+        <f t="shared" si="15"/>
         <v>1584.4896884932225</v>
       </c>
-      <c r="U15" s="231">
+      <c r="U15" s="230">
         <v>2.3290961877330481</v>
       </c>
-      <c r="V15" s="231">
-        <f t="shared" si="1"/>
+      <c r="V15" s="230">
+        <f t="shared" si="12"/>
         <v>2.3290961877330481</v>
       </c>
       <c r="W15" s="185">
@@ -36088,68 +36232,80 @@
       <c r="Y15" s="180">
         <v>1.5626820600991163</v>
       </c>
-      <c r="Z15" s="188">
+      <c r="Z15" s="180">
+        <v>0.93775040881506966</v>
+      </c>
+      <c r="AA15" s="181">
+        <v>1.9036125497719851</v>
+      </c>
+      <c r="AB15" s="188">
         <v>1.5445884513002417</v>
       </c>
-      <c r="AA15" s="180">
+      <c r="AC15" s="180">
         <v>3.4332945165733397</v>
       </c>
-      <c r="AB15" s="180">
+      <c r="AD15" s="180">
         <v>1.5626820600991163</v>
       </c>
-      <c r="AC15" s="70">
-        <f>K15*$Z15</f>
+      <c r="AE15" s="180">
+        <v>0.93775040881506966</v>
+      </c>
+      <c r="AF15" s="181">
+        <v>1.9036125497719851</v>
+      </c>
+      <c r="AG15" s="70">
+        <f t="shared" si="0"/>
         <v>33.363110548085224</v>
       </c>
-      <c r="AD15" s="8">
-        <f>L15*$Z15</f>
+      <c r="AH15" s="8">
+        <f t="shared" si="1"/>
         <v>676.95589362321959</v>
-      </c>
-      <c r="AE15" s="8">
-        <f>M15*$Z15</f>
-        <v>754.97382859262029</v>
-      </c>
-      <c r="AF15" s="8">
-        <f>N15*$Z15</f>
-        <v>1160.9273535875491</v>
-      </c>
-      <c r="AG15" s="8">
-        <f>O15*$Z15</f>
-        <v>96.163813648525405</v>
-      </c>
-      <c r="AH15" s="8">
-        <f>P15*$Z15</f>
-        <v>1166.7359999999999</v>
       </c>
       <c r="AI15" s="8">
         <f t="shared" si="2"/>
+        <v>754.97382859262029</v>
+      </c>
+      <c r="AJ15" s="8">
+        <f t="shared" si="3"/>
+        <v>1160.9273535875491</v>
+      </c>
+      <c r="AK15" s="8">
+        <f t="shared" si="4"/>
+        <v>96.163813648525405</v>
+      </c>
+      <c r="AL15" s="8">
+        <f t="shared" si="5"/>
+        <v>1166.7359999999999</v>
+      </c>
+      <c r="AM15" s="8">
+        <f t="shared" si="13"/>
         <v>3889.12</v>
       </c>
-      <c r="AJ15" s="8">
-        <f>R15*$Z15</f>
+      <c r="AN15" s="8">
+        <f t="shared" si="6"/>
         <v>106.56873540235925</v>
       </c>
-      <c r="AK15" s="8">
-        <f>S15*$Z15</f>
+      <c r="AO15" s="8">
+        <f t="shared" si="7"/>
         <v>1335.1667905466918</v>
       </c>
-      <c r="AL15" s="18">
-        <f>T15*$Z15</f>
+      <c r="AP15" s="18">
+        <f t="shared" si="8"/>
         <v>2447.3844740509489</v>
       </c>
-      <c r="AM15" s="70">
-        <f>R15*AA15</f>
+      <c r="AQ15" s="70">
+        <f t="shared" si="9"/>
         <v>236.87983332199209</v>
       </c>
-      <c r="AN15" s="217">
-        <f>(S15+T15)*AB15</f>
+      <c r="AR15" s="217">
+        <f t="shared" si="10"/>
         <v>3826.8608040000004</v>
       </c>
-      <c r="AR15" s="8"/>
-      <c r="AS15" s="8"/>
-      <c r="AT15" s="8"/>
+      <c r="AV15" s="8"/>
+      <c r="AW15" s="8"/>
+      <c r="AX15" s="8"/>
     </row>
-    <row r="16" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>21</v>
       </c>
@@ -36192,11 +36348,11 @@
         <v>0</v>
       </c>
       <c r="P16" s="39">
-        <f t="shared" si="0"/>
+        <f t="shared" si="11"/>
         <v>37.804052934905307</v>
       </c>
       <c r="Q16" s="39">
-        <f t="shared" si="3"/>
+        <f t="shared" si="14"/>
         <v>126.0135097830177</v>
       </c>
       <c r="R16" s="180">
@@ -36206,14 +36362,14 @@
         <v>26.507200357142853</v>
       </c>
       <c r="T16" s="181">
-        <f t="shared" si="4"/>
+        <f t="shared" si="15"/>
         <v>89.285442500000016</v>
       </c>
-      <c r="U16" s="231">
+      <c r="U16" s="230">
         <v>3.0330707866414395</v>
       </c>
-      <c r="V16" s="231">
-        <f t="shared" si="1"/>
+      <c r="V16" s="230">
+        <f t="shared" si="12"/>
         <v>3.0330707866414395</v>
       </c>
       <c r="W16" s="185">
@@ -36225,68 +36381,80 @@
       <c r="Y16" s="180">
         <v>2.5241716640028318</v>
       </c>
-      <c r="Z16" s="188">
+      <c r="Z16" s="180">
+        <v>5.1491548772037836</v>
+      </c>
+      <c r="AA16" s="181">
+        <v>1.7448625849617077</v>
+      </c>
+      <c r="AB16" s="188">
         <v>2.4882252747336446</v>
       </c>
-      <c r="AA16" s="180">
+      <c r="AC16" s="180">
         <v>2.0809334623226734</v>
       </c>
-      <c r="AB16" s="180">
+      <c r="AD16" s="180">
         <v>2.5241716640028318</v>
       </c>
-      <c r="AC16" s="70">
-        <f>K16*$Z16</f>
+      <c r="AE16" s="180">
+        <v>5.1491548772037836</v>
+      </c>
+      <c r="AF16" s="181">
+        <v>1.7448625849617077</v>
+      </c>
+      <c r="AG16" s="70">
+        <f t="shared" si="0"/>
         <v>14.126667214419102</v>
       </c>
-      <c r="AD16" s="8">
-        <f>L16*$Z16</f>
+      <c r="AH16" s="8">
+        <f t="shared" si="1"/>
         <v>7.6797828992016575</v>
-      </c>
-      <c r="AE16" s="8">
-        <f>M16*$Z16</f>
-        <v>9.9966938637698899</v>
-      </c>
-      <c r="AF16" s="8">
-        <f>N16*$Z16</f>
-        <v>187.68185602260934</v>
-      </c>
-      <c r="AG16" s="8">
-        <f>O16*$Z16</f>
-        <v>0</v>
-      </c>
-      <c r="AH16" s="8">
-        <f>P16*$Z16</f>
-        <v>94.064999999999998</v>
       </c>
       <c r="AI16" s="8">
         <f t="shared" si="2"/>
+        <v>9.9966938637698899</v>
+      </c>
+      <c r="AJ16" s="8">
+        <f t="shared" si="3"/>
+        <v>187.68185602260934</v>
+      </c>
+      <c r="AK16" s="8">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="AL16" s="8">
+        <f t="shared" si="5"/>
+        <v>94.064999999999998</v>
+      </c>
+      <c r="AM16" s="8">
+        <f t="shared" si="13"/>
         <v>313.55</v>
       </c>
-      <c r="AJ16" s="8">
-        <f>R16*$Z16</f>
+      <c r="AN16" s="8">
+        <f t="shared" si="6"/>
         <v>25.431819414650914</v>
       </c>
-      <c r="AK16" s="8">
-        <f>S16*$Z16</f>
+      <c r="AO16" s="8">
+        <f t="shared" si="7"/>
         <v>65.955885891071546</v>
       </c>
-      <c r="AL16" s="18">
-        <f>T16*$Z16</f>
+      <c r="AP16" s="18">
+        <f t="shared" si="8"/>
         <v>222.16229469427756</v>
       </c>
-      <c r="AM16" s="70">
-        <f>R16*AA16</f>
+      <c r="AQ16" s="70">
+        <f t="shared" si="9"/>
         <v>21.268944000000001</v>
       </c>
-      <c r="AN16" s="217">
-        <f>(S16+T16)*AB16</f>
+      <c r="AR16" s="217">
+        <f t="shared" si="10"/>
         <v>292.28050799999994</v>
       </c>
-      <c r="AR16" s="8"/>
-      <c r="AS16" s="8"/>
-      <c r="AT16" s="8"/>
+      <c r="AV16" s="8"/>
+      <c r="AW16" s="8"/>
+      <c r="AX16" s="8"/>
     </row>
-    <row r="17" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
         <v>22</v>
       </c>
@@ -36329,7 +36497,7 @@
         <v>0</v>
       </c>
       <c r="P17" s="39">
-        <f t="shared" si="0"/>
+        <f t="shared" si="11"/>
         <v>439.44768704377276</v>
       </c>
       <c r="Q17" s="39">
@@ -36343,14 +36511,14 @@
         <v>366.98680053571428</v>
       </c>
       <c r="T17" s="181">
-        <f t="shared" si="4"/>
+        <f t="shared" si="15"/>
         <v>1051.0202005930955</v>
       </c>
-      <c r="U17" s="231">
+      <c r="U17" s="230">
         <v>3.873164145810307</v>
       </c>
-      <c r="V17" s="231">
-        <f t="shared" si="1"/>
+      <c r="V17" s="230">
+        <f t="shared" si="12"/>
         <v>3.873164145810307</v>
       </c>
       <c r="W17" s="185">
@@ -36362,68 +36530,80 @@
       <c r="Y17" s="180">
         <v>2.3438878012267899</v>
       </c>
-      <c r="Z17" s="188">
+      <c r="Z17" s="180">
+        <v>0.49615934887630941</v>
+      </c>
+      <c r="AA17" s="181">
+        <v>3.2219068845946852</v>
+      </c>
+      <c r="AB17" s="188">
         <v>2.8033372539248047</v>
       </c>
-      <c r="AA17" s="180">
+      <c r="AC17" s="180">
         <v>4.9032250945307521</v>
       </c>
-      <c r="AB17" s="180">
+      <c r="AD17" s="180">
         <v>2.3438878012267899</v>
       </c>
-      <c r="AC17" s="70">
-        <f>K17*$Z17</f>
+      <c r="AE17" s="180">
+        <v>2.1152391169621825</v>
+      </c>
+      <c r="AF17" s="181">
+        <v>3.2219068845946852</v>
+      </c>
+      <c r="AG17" s="70">
+        <f t="shared" si="0"/>
         <v>103.85225371608249</v>
       </c>
-      <c r="AD17" s="8">
-        <f>L17*$Z17</f>
+      <c r="AH17" s="8">
+        <f t="shared" si="1"/>
         <v>259.57080802128644</v>
       </c>
-      <c r="AE17" s="8">
-        <f>M17*$Z17</f>
+      <c r="AI17" s="8">
+        <f t="shared" si="2"/>
         <v>1027.0867030929699</v>
       </c>
-      <c r="AF17" s="8">
-        <f>N17*$Z17</f>
+      <c r="AJ17" s="8">
+        <f t="shared" si="3"/>
         <v>1483.9704037317538</v>
       </c>
-      <c r="AG17" s="8">
-        <f>O17*$Z17</f>
+      <c r="AK17" s="8">
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="AH17" s="8">
-        <f>P17*$Z17</f>
+      <c r="AL17" s="8">
+        <f t="shared" si="5"/>
         <v>1231.9200722408968</v>
       </c>
-      <c r="AI17" s="8">
-        <f>AJ17+AK17+AL17</f>
+      <c r="AM17" s="8">
+        <f>AN17+AO17+AP17</f>
         <v>4106.4002408029901</v>
       </c>
-      <c r="AJ17" s="8">
-        <f>R17*$Z17</f>
+      <c r="AN17" s="8">
+        <f t="shared" si="6"/>
         <v>131.24838821240454</v>
       </c>
-      <c r="AK17" s="8">
-        <f>S17*$Z17</f>
+      <c r="AO17" s="8">
+        <f t="shared" si="7"/>
         <v>1028.7877696404394</v>
       </c>
-      <c r="AL17" s="18">
-        <f>T17*$Z17</f>
+      <c r="AP17" s="18">
+        <f t="shared" si="8"/>
         <v>2946.364082950146</v>
       </c>
-      <c r="AM17" s="70">
-        <f>R17*AA17</f>
+      <c r="AQ17" s="70">
+        <f t="shared" si="9"/>
         <v>229.56224400000002</v>
       </c>
-      <c r="AN17" s="217">
-        <f>(S17+T17)*AB17</f>
+      <c r="AR17" s="217">
+        <f t="shared" si="10"/>
         <v>3323.6493120000005</v>
       </c>
-      <c r="AR17" s="8"/>
-      <c r="AS17" s="8"/>
-      <c r="AT17" s="8"/>
+      <c r="AV17" s="8"/>
+      <c r="AW17" s="8"/>
+      <c r="AX17" s="8"/>
     </row>
-    <row r="18" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
         <v>23</v>
       </c>
@@ -36466,11 +36646,11 @@
         <v>420.75</v>
       </c>
       <c r="P18" s="39">
-        <f t="shared" si="0"/>
+        <f t="shared" si="11"/>
         <v>343.34627599084405</v>
       </c>
       <c r="Q18" s="39">
-        <f t="shared" si="3"/>
+        <f t="shared" si="14"/>
         <v>1144.4875866361469</v>
       </c>
       <c r="R18" s="180">
@@ -36480,14 +36660,14 @@
         <v>415.71572499999996</v>
       </c>
       <c r="T18" s="181">
-        <f t="shared" si="4"/>
+        <f t="shared" si="15"/>
         <v>653.95909529976166</v>
       </c>
-      <c r="U18" s="231">
+      <c r="U18" s="230">
         <v>2.4735851208160708</v>
       </c>
-      <c r="V18" s="231">
-        <f t="shared" si="1"/>
+      <c r="V18" s="230">
+        <f t="shared" si="12"/>
         <v>2.4735851208160708</v>
       </c>
       <c r="W18" s="185">
@@ -36499,69 +36679,81 @@
       <c r="Y18" s="180">
         <v>2.5928476013137933</v>
       </c>
-      <c r="Z18" s="188">
+      <c r="Z18" s="180">
+        <v>1.7738590090620221</v>
+      </c>
+      <c r="AA18" s="181">
+        <v>1.6235655225452563</v>
+      </c>
+      <c r="AB18" s="188">
         <f>W18</f>
         <v>2.1045803101102205</v>
       </c>
-      <c r="AA18" s="180">
+      <c r="AC18" s="180">
         <v>2.546348829602767</v>
       </c>
-      <c r="AB18" s="180">
+      <c r="AD18" s="180">
         <v>2.5928476013137933</v>
       </c>
-      <c r="AC18" s="70">
-        <f>K18*$Z18</f>
+      <c r="AE18" s="180">
+        <v>1.7738590090620221</v>
+      </c>
+      <c r="AF18" s="181">
+        <v>1.6235655225452563</v>
+      </c>
+      <c r="AG18" s="70">
+        <f t="shared" si="0"/>
         <v>41.831976010339446</v>
       </c>
-      <c r="AD18" s="8">
-        <f>L18*$Z18</f>
+      <c r="AH18" s="8">
+        <f t="shared" si="1"/>
         <v>9.743522847209535</v>
-      </c>
-      <c r="AE18" s="8">
-        <f>M18*$Z18</f>
-        <v>0</v>
-      </c>
-      <c r="AF18" s="8">
-        <f>N18*$Z18</f>
-        <v>748.98856366357586</v>
-      </c>
-      <c r="AG18" s="8">
-        <f>O18*$Z18</f>
-        <v>885.50216547887533</v>
-      </c>
-      <c r="AH18" s="8">
-        <f>P18*$Z18</f>
-        <v>722.59981199999993</v>
       </c>
       <c r="AI18" s="8">
         <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="AJ18" s="8">
+        <f t="shared" si="3"/>
+        <v>748.98856366357586</v>
+      </c>
+      <c r="AK18" s="8">
+        <f t="shared" si="4"/>
+        <v>885.50216547887533</v>
+      </c>
+      <c r="AL18" s="8">
+        <f t="shared" si="5"/>
+        <v>722.59981199999993</v>
+      </c>
+      <c r="AM18" s="8">
+        <f t="shared" si="13"/>
         <v>2408.6660400000001</v>
       </c>
-      <c r="AJ18" s="8">
-        <f>R18*$Z18</f>
+      <c r="AN18" s="8">
+        <f t="shared" si="6"/>
         <v>157.44947497643327</v>
       </c>
-      <c r="AK18" s="8">
-        <f>S18*$Z18</f>
+      <c r="AO18" s="8">
+        <f t="shared" si="7"/>
         <v>874.90712943819506</v>
       </c>
-      <c r="AL18" s="18">
-        <f>T18*$Z18</f>
+      <c r="AP18" s="18">
+        <f t="shared" si="8"/>
         <v>1376.3094355853716</v>
       </c>
-      <c r="AM18" s="70">
-        <f>R18*AA18</f>
+      <c r="AQ18" s="70">
+        <f t="shared" si="9"/>
         <v>190.49940000000001</v>
       </c>
-      <c r="AN18" s="217">
-        <f>(S18+T18)*AB18</f>
+      <c r="AR18" s="217">
+        <f t="shared" si="10"/>
         <v>2773.503792</v>
       </c>
-      <c r="AR18" s="8"/>
-      <c r="AS18" s="8"/>
-      <c r="AT18" s="8"/>
+      <c r="AV18" s="8"/>
+      <c r="AW18" s="8"/>
+      <c r="AX18" s="8"/>
     </row>
-    <row r="19" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
         <v>24</v>
       </c>
@@ -36604,11 +36796,11 @@
         <v>682.85249999999996</v>
       </c>
       <c r="P19" s="39">
-        <f t="shared" si="0"/>
+        <f t="shared" si="11"/>
         <v>1666.7249785714284</v>
       </c>
       <c r="Q19" s="39">
-        <f t="shared" si="3"/>
+        <f t="shared" si="14"/>
         <v>5555.7499285714284</v>
       </c>
       <c r="R19" s="180">
@@ -36618,14 +36810,14 @@
         <v>1235.1539360714287</v>
       </c>
       <c r="T19" s="181">
-        <f t="shared" si="4"/>
+        <f t="shared" si="15"/>
         <v>4128.6955639285716</v>
       </c>
-      <c r="U19" s="231">
+      <c r="U19" s="230">
         <v>1.7483888095078277</v>
       </c>
-      <c r="V19" s="231">
-        <f t="shared" si="1"/>
+      <c r="V19" s="230">
+        <f t="shared" si="12"/>
         <v>1.7483888095078277</v>
       </c>
       <c r="W19" s="185">
@@ -36637,68 +36829,80 @@
       <c r="Y19" s="180">
         <v>1.3708564157141245</v>
       </c>
-      <c r="Z19" s="188">
+      <c r="Z19" s="180">
+        <v>2.1464590660112517</v>
+      </c>
+      <c r="AA19" s="181">
+        <v>1.1388246149895453</v>
+      </c>
+      <c r="AB19" s="188">
         <v>1.4023615353766246</v>
       </c>
-      <c r="AA19" s="180">
+      <c r="AC19" s="180">
         <v>2.2829899613117819</v>
       </c>
-      <c r="AB19" s="180">
+      <c r="AD19" s="180">
         <v>1.3708564157141245</v>
       </c>
-      <c r="AC19" s="70">
-        <f>K19*$Z19</f>
+      <c r="AE19" s="180">
+        <v>2.1464590660112517</v>
+      </c>
+      <c r="AF19" s="181">
+        <v>1.1388246149895453</v>
+      </c>
+      <c r="AG19" s="70">
+        <f t="shared" si="0"/>
         <v>106.72532228830264</v>
       </c>
-      <c r="AD19" s="8">
-        <f>L19*$Z19</f>
+      <c r="AH19" s="8">
+        <f t="shared" si="1"/>
         <v>264.02744441265418</v>
-      </c>
-      <c r="AE19" s="8">
-        <f>M19*$Z19</f>
-        <v>595.21833007525458</v>
-      </c>
-      <c r="AF19" s="8">
-        <f>N19*$Z19</f>
-        <v>3530.2418228880229</v>
-      </c>
-      <c r="AG19" s="8">
-        <f>O19*$Z19</f>
-        <v>957.60608033576648</v>
-      </c>
-      <c r="AH19" s="8">
-        <f>P19*$Z19</f>
-        <v>2337.3510000000001</v>
       </c>
       <c r="AI19" s="8">
         <f t="shared" si="2"/>
+        <v>595.21833007525458</v>
+      </c>
+      <c r="AJ19" s="8">
+        <f t="shared" si="3"/>
+        <v>3530.2418228880229</v>
+      </c>
+      <c r="AK19" s="8">
+        <f t="shared" si="4"/>
+        <v>957.60608033576648</v>
+      </c>
+      <c r="AL19" s="8">
+        <f t="shared" si="5"/>
+        <v>2337.3510000000001</v>
+      </c>
+      <c r="AM19" s="8">
+        <f t="shared" si="13"/>
         <v>7791.170000000001</v>
       </c>
-      <c r="AJ19" s="8">
-        <f>R19*$Z19</f>
+      <c r="AN19" s="8">
+        <f t="shared" si="6"/>
         <v>269.11377965086081</v>
       </c>
-      <c r="AK19" s="8">
-        <f>S19*$Z19</f>
+      <c r="AO19" s="8">
+        <f t="shared" si="7"/>
         <v>1732.1323702156099</v>
       </c>
-      <c r="AL19" s="18">
-        <f>T19*$Z19</f>
+      <c r="AP19" s="18">
+        <f t="shared" si="8"/>
         <v>5789.9238501335303</v>
       </c>
-      <c r="AM19" s="70">
-        <f>R19*AA19</f>
+      <c r="AQ19" s="70">
+        <f t="shared" si="9"/>
         <v>438.10675200000009</v>
       </c>
-      <c r="AN19" s="217">
-        <f>(S19+T19)*AB19</f>
+      <c r="AR19" s="217">
+        <f t="shared" si="10"/>
         <v>7353.0674999999992</v>
       </c>
-      <c r="AR19" s="8"/>
-      <c r="AS19" s="8"/>
-      <c r="AT19" s="8"/>
+      <c r="AV19" s="8"/>
+      <c r="AW19" s="8"/>
+      <c r="AX19" s="8"/>
     </row>
-    <row r="20" spans="1:46" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:50" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="26" t="s">
         <v>25</v>
       </c>
@@ -36741,11 +36945,11 @@
         <v>519.51137754317494</v>
       </c>
       <c r="P20" s="40">
-        <f t="shared" si="0"/>
+        <f t="shared" si="11"/>
         <v>902.8282649015764</v>
       </c>
       <c r="Q20" s="40">
-        <f t="shared" si="3"/>
+        <f t="shared" si="14"/>
         <v>3009.4275496719215</v>
       </c>
       <c r="R20" s="65">
@@ -36755,14 +36959,14 @@
         <v>619.13960072678344</v>
       </c>
       <c r="T20" s="183">
-        <f t="shared" si="4"/>
+        <f t="shared" si="15"/>
         <v>2280.8389992602843</v>
       </c>
-      <c r="U20" s="232">
+      <c r="U20" s="231">
         <v>1.4060253396092017</v>
       </c>
-      <c r="V20" s="232">
-        <f t="shared" si="1"/>
+      <c r="V20" s="231">
+        <f t="shared" si="12"/>
         <v>1.4060253396092017</v>
       </c>
       <c r="W20" s="186">
@@ -36774,68 +36978,80 @@
       <c r="Y20" s="65">
         <v>1.0437769423586432</v>
       </c>
-      <c r="Z20" s="189">
+      <c r="Z20" s="65">
+        <v>1.4536889498644299</v>
+      </c>
+      <c r="AA20" s="183">
+        <v>0.93250527577342934</v>
+      </c>
+      <c r="AB20" s="189">
         <v>1.147653479937246</v>
       </c>
-      <c r="AA20" s="65">
+      <c r="AC20" s="65">
         <v>3.8999392979928231</v>
       </c>
-      <c r="AB20" s="65">
+      <c r="AD20" s="65">
         <v>1.0437769423586432</v>
       </c>
-      <c r="AC20" s="71">
-        <f>K20*$Z20</f>
+      <c r="AE20" s="65">
+        <v>1.4536889498644299</v>
+      </c>
+      <c r="AF20" s="183">
+        <v>1.7375621622004116</v>
+      </c>
+      <c r="AG20" s="71">
+        <f t="shared" si="0"/>
         <v>53.627551810507633</v>
       </c>
-      <c r="AD20" s="22">
-        <f>L20*$Z20</f>
+      <c r="AH20" s="22">
+        <f t="shared" si="1"/>
         <v>60.216976413589322</v>
-      </c>
-      <c r="AE20" s="22">
-        <f>M20*$Z20</f>
-        <v>244.29870096728166</v>
-      </c>
-      <c r="AF20" s="22">
-        <f>N20*$Z20</f>
-        <v>1463.283730504204</v>
-      </c>
-      <c r="AG20" s="22">
-        <f>O20*$Z20</f>
-        <v>596.21904030441715</v>
-      </c>
-      <c r="AH20" s="22">
-        <f>P20*$Z20</f>
-        <v>1036.134</v>
       </c>
       <c r="AI20" s="22">
         <f t="shared" si="2"/>
+        <v>244.29870096728166</v>
+      </c>
+      <c r="AJ20" s="22">
+        <f t="shared" si="3"/>
+        <v>1463.283730504204</v>
+      </c>
+      <c r="AK20" s="22">
+        <f t="shared" si="4"/>
+        <v>596.21904030441715</v>
+      </c>
+      <c r="AL20" s="22">
+        <f t="shared" si="5"/>
+        <v>1036.134</v>
+      </c>
+      <c r="AM20" s="22">
+        <f t="shared" si="13"/>
         <v>3453.7799999999997</v>
       </c>
-      <c r="AJ20" s="22">
-        <f>R20*$Z20</f>
+      <c r="AN20" s="22">
+        <f t="shared" si="6"/>
         <v>125.60946798129885</v>
       </c>
-      <c r="AK20" s="22">
-        <f>S20*$Z20</f>
+      <c r="AO20" s="22">
+        <f t="shared" si="7"/>
         <v>710.55771734105008</v>
       </c>
-      <c r="AL20" s="23">
-        <f>T20*$Z20</f>
+      <c r="AP20" s="23">
+        <f t="shared" si="8"/>
         <v>2617.6128146776509</v>
       </c>
-      <c r="AM20" s="71">
-        <f>R20*AA20</f>
+      <c r="AQ20" s="71">
+        <f t="shared" si="9"/>
         <v>426.84426000000002</v>
       </c>
-      <c r="AN20" s="224">
-        <f>(S20+T20)*AB20</f>
+      <c r="AR20" s="224">
+        <f t="shared" si="10"/>
         <v>3026.9307960000006</v>
       </c>
-      <c r="AR20" s="8"/>
-      <c r="AS20" s="8"/>
-      <c r="AT20" s="8"/>
+      <c r="AV20" s="8"/>
+      <c r="AW20" s="8"/>
+      <c r="AX20" s="8"/>
     </row>
-    <row r="22" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:50" x14ac:dyDescent="0.25">
       <c r="R22" s="36"/>
       <c r="S22" s="41"/>
       <c r="T22" s="36"/>
@@ -36846,28 +37062,36 @@
       <c r="Z22" s="36"/>
       <c r="AA22" s="36"/>
       <c r="AB22" s="36"/>
+      <c r="AC22" s="36"/>
+      <c r="AD22" s="36"/>
+      <c r="AE22" s="36"/>
+      <c r="AF22" s="36"/>
     </row>
-    <row r="23" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:50" x14ac:dyDescent="0.25">
       <c r="R23" s="36"/>
       <c r="S23" s="42"/>
       <c r="T23" s="36"/>
       <c r="U23" s="36"/>
-      <c r="V23" s="229"/>
+      <c r="V23" s="228"/>
       <c r="W23" s="36"/>
       <c r="X23" s="39"/>
       <c r="Y23" s="39"/>
       <c r="Z23" s="39"/>
       <c r="AA23" s="39"/>
       <c r="AB23" s="39"/>
-      <c r="AC23" s="8"/>
-      <c r="AD23" s="8"/>
-      <c r="AE23" s="8"/>
-      <c r="AF23" s="8"/>
+      <c r="AC23" s="39"/>
+      <c r="AD23" s="39"/>
+      <c r="AE23" s="39"/>
+      <c r="AF23" s="39"/>
       <c r="AG23" s="8"/>
       <c r="AH23" s="8"/>
       <c r="AI23" s="8"/>
+      <c r="AJ23" s="8"/>
+      <c r="AK23" s="8"/>
+      <c r="AL23" s="8"/>
+      <c r="AM23" s="8"/>
     </row>
-    <row r="24" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:50" x14ac:dyDescent="0.25">
       <c r="P24" s="39"/>
       <c r="Q24" s="39"/>
       <c r="S24" s="39"/>
@@ -36880,15 +37104,19 @@
       <c r="Z24" s="39"/>
       <c r="AA24" s="39"/>
       <c r="AB24" s="39"/>
-      <c r="AC24" s="8"/>
-      <c r="AD24" s="8"/>
-      <c r="AE24" s="8"/>
-      <c r="AF24" s="8"/>
+      <c r="AC24" s="39"/>
+      <c r="AD24" s="39"/>
+      <c r="AE24" s="39"/>
+      <c r="AF24" s="39"/>
       <c r="AG24" s="8"/>
       <c r="AH24" s="8"/>
       <c r="AI24" s="8"/>
+      <c r="AJ24" s="8"/>
+      <c r="AK24" s="8"/>
+      <c r="AL24" s="8"/>
+      <c r="AM24" s="8"/>
     </row>
-    <row r="25" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:50" x14ac:dyDescent="0.25">
       <c r="P25" s="36"/>
       <c r="Q25" s="39"/>
       <c r="S25" s="39"/>
@@ -36899,15 +37127,19 @@
       <c r="Z25" s="39"/>
       <c r="AA25" s="39"/>
       <c r="AB25" s="39"/>
-      <c r="AC25" s="8"/>
-      <c r="AD25" s="8"/>
-      <c r="AE25" s="8"/>
-      <c r="AF25" s="8"/>
+      <c r="AC25" s="39"/>
+      <c r="AD25" s="39"/>
+      <c r="AE25" s="39"/>
+      <c r="AF25" s="39"/>
       <c r="AG25" s="8"/>
       <c r="AH25" s="8"/>
       <c r="AI25" s="8"/>
+      <c r="AJ25" s="8"/>
+      <c r="AK25" s="8"/>
+      <c r="AL25" s="8"/>
+      <c r="AM25" s="8"/>
     </row>
-    <row r="26" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:50" x14ac:dyDescent="0.25">
       <c r="R26" s="36"/>
       <c r="S26" s="42"/>
       <c r="T26" s="36"/>
@@ -36926,9 +37158,13 @@
       <c r="AG26" s="39"/>
       <c r="AH26" s="39"/>
       <c r="AI26" s="39"/>
-      <c r="AJ26" s="36"/>
+      <c r="AJ26" s="39"/>
+      <c r="AK26" s="39"/>
+      <c r="AL26" s="39"/>
+      <c r="AM26" s="39"/>
+      <c r="AN26" s="36"/>
     </row>
-    <row r="27" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:50" x14ac:dyDescent="0.25">
       <c r="R27" s="36"/>
       <c r="S27" s="42"/>
       <c r="T27" s="36"/>
@@ -36940,8 +37176,12 @@
       <c r="Z27" s="36"/>
       <c r="AA27" s="36"/>
       <c r="AB27" s="36"/>
+      <c r="AC27" s="36"/>
+      <c r="AD27" s="36"/>
+      <c r="AE27" s="36"/>
+      <c r="AF27" s="36"/>
     </row>
-    <row r="28" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:50" x14ac:dyDescent="0.25">
       <c r="P28" s="36"/>
       <c r="Q28" s="36"/>
       <c r="R28" s="36"/>
@@ -36955,8 +37195,12 @@
       <c r="Z28" s="36"/>
       <c r="AA28" s="36"/>
       <c r="AB28" s="36"/>
+      <c r="AC28" s="36"/>
+      <c r="AD28" s="36"/>
+      <c r="AE28" s="36"/>
+      <c r="AF28" s="36"/>
     </row>
-    <row r="29" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:50" x14ac:dyDescent="0.25">
       <c r="P29" s="41"/>
       <c r="Q29" s="36"/>
       <c r="R29" s="36"/>
@@ -36970,8 +37214,12 @@
       <c r="Z29" s="36"/>
       <c r="AA29" s="36"/>
       <c r="AB29" s="36"/>
+      <c r="AC29" s="36"/>
+      <c r="AD29" s="36"/>
+      <c r="AE29" s="36"/>
+      <c r="AF29" s="36"/>
     </row>
-    <row r="30" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:50" x14ac:dyDescent="0.25">
       <c r="P30" s="36"/>
       <c r="Q30" s="42"/>
       <c r="R30" s="36"/>
@@ -36985,8 +37233,12 @@
       <c r="Z30" s="36"/>
       <c r="AA30" s="36"/>
       <c r="AB30" s="36"/>
+      <c r="AC30" s="36"/>
+      <c r="AD30" s="36"/>
+      <c r="AE30" s="36"/>
+      <c r="AF30" s="36"/>
     </row>
-    <row r="31" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:50" x14ac:dyDescent="0.25">
       <c r="P31" s="36"/>
       <c r="Q31" s="42"/>
       <c r="R31" s="36"/>
@@ -37000,8 +37252,12 @@
       <c r="Z31" s="36"/>
       <c r="AA31" s="36"/>
       <c r="AB31" s="36"/>
+      <c r="AC31" s="36"/>
+      <c r="AD31" s="36"/>
+      <c r="AE31" s="36"/>
+      <c r="AF31" s="36"/>
     </row>
-    <row r="32" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:50" x14ac:dyDescent="0.25">
       <c r="R32" s="36"/>
       <c r="S32" s="42"/>
       <c r="T32" s="36"/>
@@ -37013,8 +37269,12 @@
       <c r="Z32" s="36"/>
       <c r="AA32" s="36"/>
       <c r="AB32" s="36"/>
+      <c r="AC32" s="36"/>
+      <c r="AD32" s="36"/>
+      <c r="AE32" s="36"/>
+      <c r="AF32" s="36"/>
     </row>
-    <row r="33" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:39" x14ac:dyDescent="0.25">
       <c r="R33" s="36"/>
       <c r="S33" s="42"/>
       <c r="T33" s="36"/>
@@ -37026,8 +37286,12 @@
       <c r="Z33" s="36"/>
       <c r="AA33" s="36"/>
       <c r="AB33" s="36"/>
+      <c r="AC33" s="36"/>
+      <c r="AD33" s="36"/>
+      <c r="AE33" s="36"/>
+      <c r="AF33" s="36"/>
     </row>
-    <row r="34" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:39" x14ac:dyDescent="0.25">
       <c r="R34" s="36"/>
       <c r="S34" s="42"/>
       <c r="T34" s="36"/>
@@ -37039,8 +37303,12 @@
       <c r="Z34" s="36"/>
       <c r="AA34" s="36"/>
       <c r="AB34" s="36"/>
+      <c r="AC34" s="36"/>
+      <c r="AD34" s="36"/>
+      <c r="AE34" s="36"/>
+      <c r="AF34" s="36"/>
     </row>
-    <row r="35" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:39" x14ac:dyDescent="0.25">
       <c r="R35" s="36"/>
       <c r="S35" s="42"/>
       <c r="T35" s="36"/>
@@ -37052,9 +37320,13 @@
       <c r="Z35" s="36"/>
       <c r="AA35" s="36"/>
       <c r="AB35" s="36"/>
-      <c r="AI35" s="43"/>
+      <c r="AC35" s="36"/>
+      <c r="AD35" s="36"/>
+      <c r="AE35" s="36"/>
+      <c r="AF35" s="36"/>
+      <c r="AM35" s="43"/>
     </row>
-    <row r="36" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A36" s="66"/>
       <c r="B36" s="66"/>
       <c r="C36" s="66"/>
@@ -37072,9 +37344,9 @@
       <c r="U36" s="36"/>
       <c r="V36" s="8"/>
       <c r="W36" s="8"/>
-      <c r="Z36" s="36"/>
+      <c r="AB36" s="36"/>
     </row>
-    <row r="37" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A37" s="66"/>
       <c r="B37" s="66"/>
       <c r="C37" s="66"/>
@@ -37093,7 +37365,7 @@
       <c r="V37" s="8"/>
       <c r="W37" s="8"/>
     </row>
-    <row r="38" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A38" s="66"/>
       <c r="B38" s="66"/>
       <c r="C38" s="66"/>
@@ -37112,7 +37384,7 @@
       <c r="V38" s="8"/>
       <c r="W38" s="8"/>
     </row>
-    <row r="39" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A39" s="66"/>
       <c r="B39" s="66"/>
       <c r="C39" s="66"/>
@@ -37130,7 +37402,7 @@
       <c r="V39" s="8"/>
       <c r="W39" s="8"/>
     </row>
-    <row r="40" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A40" s="66"/>
       <c r="B40" s="66"/>
       <c r="C40" s="66"/>
@@ -37148,7 +37420,7 @@
       <c r="V40" s="8"/>
       <c r="W40" s="8"/>
     </row>
-    <row r="41" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A41" s="66"/>
       <c r="B41" s="66"/>
       <c r="C41" s="66"/>
@@ -37166,7 +37438,7 @@
       <c r="V41" s="8"/>
       <c r="W41" s="8"/>
     </row>
-    <row r="42" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A42" s="66"/>
       <c r="B42" s="66"/>
       <c r="C42" s="66"/>
@@ -37184,7 +37456,7 @@
       <c r="V42" s="8"/>
       <c r="W42" s="8"/>
     </row>
-    <row r="43" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A43" s="66"/>
       <c r="B43" s="66"/>
       <c r="C43" s="66"/>
@@ -37202,27 +37474,27 @@
       <c r="V43" s="8"/>
       <c r="W43" s="8"/>
     </row>
-    <row r="44" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:39" x14ac:dyDescent="0.25">
       <c r="I44" s="66"/>
       <c r="K44" s="67"/>
       <c r="V44" s="8"/>
       <c r="W44" s="8"/>
     </row>
-    <row r="45" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:39" x14ac:dyDescent="0.25">
       <c r="I45" s="66"/>
       <c r="K45" s="67"/>
       <c r="V45" s="8"/>
       <c r="W45" s="8"/>
     </row>
-    <row r="46" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:39" x14ac:dyDescent="0.25">
       <c r="I46" s="66"/>
       <c r="K46" s="67"/>
     </row>
-    <row r="47" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:39" x14ac:dyDescent="0.25">
       <c r="I47" s="66"/>
       <c r="K47" s="67"/>
     </row>
-    <row r="48" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:39" x14ac:dyDescent="0.25">
       <c r="I48" s="66"/>
       <c r="K48" s="67"/>
     </row>
@@ -37244,19 +37516,19 @@
     </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="AC4:AL4"/>
-    <mergeCell ref="AC1:AL1"/>
-    <mergeCell ref="AM1:AN1"/>
-    <mergeCell ref="AM4:AN4"/>
+    <mergeCell ref="AG4:AP4"/>
+    <mergeCell ref="AG1:AP1"/>
+    <mergeCell ref="AQ1:AR1"/>
+    <mergeCell ref="AQ4:AR4"/>
     <mergeCell ref="B1:J1"/>
     <mergeCell ref="B4:J4"/>
     <mergeCell ref="W4:Y4"/>
-    <mergeCell ref="Z4:AB4"/>
-    <mergeCell ref="W2:Y2"/>
-    <mergeCell ref="Z2:AB2"/>
-    <mergeCell ref="U1:AB1"/>
+    <mergeCell ref="AB4:AD4"/>
     <mergeCell ref="K1:T1"/>
     <mergeCell ref="K4:T4"/>
+    <mergeCell ref="W2:AA2"/>
+    <mergeCell ref="AB2:AF2"/>
+    <mergeCell ref="U1:AF1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78749999999999998" bottom="0.78749999999999998" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -37283,11 +37555,11 @@
   <sheetData>
     <row r="1" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A1" s="38"/>
-      <c r="B1" s="243" t="s">
+      <c r="B1" s="242" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="244"/>
-      <c r="D1" s="245"/>
+      <c r="C1" s="243"/>
+      <c r="D1" s="244"/>
       <c r="E1" s="225" t="s">
         <v>89</v>
       </c>
@@ -37332,16 +37604,16 @@
       <c r="A4" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="B4" s="262" t="s">
+      <c r="B4" s="261" t="s">
         <v>8</v>
       </c>
-      <c r="C4" s="263"/>
-      <c r="D4" s="264"/>
-      <c r="E4" s="253" t="s">
+      <c r="C4" s="262"/>
+      <c r="D4" s="263"/>
+      <c r="E4" s="252" t="s">
         <v>8</v>
       </c>
-      <c r="F4" s="261"/>
-      <c r="G4" s="254"/>
+      <c r="F4" s="260"/>
+      <c r="G4" s="253"/>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="195" t="s">
@@ -37360,15 +37632,15 @@
         <v>1462.2272874831046</v>
       </c>
       <c r="E5" s="8">
-        <f>'Iron&amp;Steel'!W5+'Non-Ferrous'!AC5+'Non-metallic Minerals'!Z5+'Paper&amp;Pulp'!AF5+Chemicals!AI5</f>
+        <f>'Iron&amp;Steel'!W5+'Non-Ferrous'!AC5+'Non-metallic Minerals'!Z5+'Paper&amp;Pulp'!AF5+Chemicals!AM5</f>
         <v>2387.1038582690062</v>
       </c>
       <c r="F5" s="8">
-        <f>'Iron&amp;Steel'!Z5+'Non-Ferrous'!AF5+'Non-metallic Minerals'!AC5+'Paper&amp;Pulp'!AI5+Chemicals!AM5</f>
+        <f>'Iron&amp;Steel'!Z5+'Non-Ferrous'!AF5+'Non-metallic Minerals'!AC5+'Paper&amp;Pulp'!AI5+Chemicals!AQ5</f>
         <v>414.04958910992082</v>
       </c>
       <c r="G5" s="18">
-        <f>'Iron&amp;Steel'!AA5+'Non-Ferrous'!AG5+'Non-metallic Minerals'!AD5+'Paper&amp;Pulp'!AJ5+Chemicals!AN5</f>
+        <f>'Iron&amp;Steel'!AA5+'Non-Ferrous'!AG5+'Non-metallic Minerals'!AD5+'Paper&amp;Pulp'!AJ5+Chemicals!AR5</f>
         <v>2097.8612472660971</v>
       </c>
       <c r="H5" s="8"/>
@@ -37390,15 +37662,15 @@
         <v>353.18550057646036</v>
       </c>
       <c r="E6" s="8">
-        <f>'Iron&amp;Steel'!W6+'Non-Ferrous'!AC6+'Non-metallic Minerals'!Z6+'Paper&amp;Pulp'!AF6+Chemicals!AI6</f>
+        <f>'Iron&amp;Steel'!W6+'Non-Ferrous'!AC6+'Non-metallic Minerals'!Z6+'Paper&amp;Pulp'!AF6+Chemicals!AM6</f>
         <v>902.40790025046022</v>
       </c>
       <c r="F6" s="8">
-        <f>'Iron&amp;Steel'!Z6+'Non-Ferrous'!AF6+'Non-metallic Minerals'!AC6+'Paper&amp;Pulp'!AI6+Chemicals!AM6</f>
+        <f>'Iron&amp;Steel'!Z6+'Non-Ferrous'!AF6+'Non-metallic Minerals'!AC6+'Paper&amp;Pulp'!AI6+Chemicals!AQ6</f>
         <v>215.49954005900983</v>
       </c>
       <c r="G6" s="18">
-        <f>'Iron&amp;Steel'!AA6+'Non-Ferrous'!AG6+'Non-metallic Minerals'!AD6+'Paper&amp;Pulp'!AJ6+Chemicals!AN6</f>
+        <f>'Iron&amp;Steel'!AA6+'Non-Ferrous'!AG6+'Non-metallic Minerals'!AD6+'Paper&amp;Pulp'!AJ6+Chemicals!AR6</f>
         <v>686.97736545768043</v>
       </c>
     </row>
@@ -37419,15 +37691,15 @@
         <v>1107.5808104885709</v>
       </c>
       <c r="E7" s="8">
-        <f>'Iron&amp;Steel'!W7+'Non-Ferrous'!AC7+'Non-metallic Minerals'!Z7+'Paper&amp;Pulp'!AF7+Chemicals!AI7</f>
+        <f>'Iron&amp;Steel'!W7+'Non-Ferrous'!AC7+'Non-metallic Minerals'!Z7+'Paper&amp;Pulp'!AF7+Chemicals!AM7</f>
         <v>1866.2447280271999</v>
       </c>
       <c r="F7" s="8">
-        <f>'Iron&amp;Steel'!Z7+'Non-Ferrous'!AF7+'Non-metallic Minerals'!AC7+'Paper&amp;Pulp'!AI7+Chemicals!AM7</f>
+        <f>'Iron&amp;Steel'!Z7+'Non-Ferrous'!AF7+'Non-metallic Minerals'!AC7+'Paper&amp;Pulp'!AI7+Chemicals!AQ7</f>
         <v>473.77828800000049</v>
       </c>
       <c r="G7" s="18">
-        <f>'Iron&amp;Steel'!AA7+'Non-Ferrous'!AG7+'Non-metallic Minerals'!AD7+'Paper&amp;Pulp'!AJ7+Chemicals!AN7</f>
+        <f>'Iron&amp;Steel'!AA7+'Non-Ferrous'!AG7+'Non-metallic Minerals'!AD7+'Paper&amp;Pulp'!AJ7+Chemicals!AR7</f>
         <v>1392.4652200271998</v>
       </c>
     </row>
@@ -37448,15 +37720,15 @@
         <v>31999.995107042709</v>
       </c>
       <c r="E8" s="8">
-        <f>'Iron&amp;Steel'!W8+'Non-Ferrous'!AC8+'Non-metallic Minerals'!Z8+'Paper&amp;Pulp'!AF8+Chemicals!AI8</f>
+        <f>'Iron&amp;Steel'!W8+'Non-Ferrous'!AC8+'Non-metallic Minerals'!Z8+'Paper&amp;Pulp'!AF8+Chemicals!AM8</f>
         <v>41462.707595764863</v>
       </c>
       <c r="F8" s="8">
-        <f>'Iron&amp;Steel'!Z8+'Non-Ferrous'!AF8+'Non-metallic Minerals'!AC8+'Paper&amp;Pulp'!AI8+Chemicals!AM8</f>
+        <f>'Iron&amp;Steel'!Z8+'Non-Ferrous'!AF8+'Non-metallic Minerals'!AC8+'Paper&amp;Pulp'!AI8+Chemicals!AQ8</f>
         <v>8288.5660919999955</v>
       </c>
       <c r="G8" s="18">
-        <f>'Iron&amp;Steel'!AA8+'Non-Ferrous'!AG8+'Non-metallic Minerals'!AD8+'Paper&amp;Pulp'!AJ8+Chemicals!AN8</f>
+        <f>'Iron&amp;Steel'!AA8+'Non-Ferrous'!AG8+'Non-metallic Minerals'!AD8+'Paper&amp;Pulp'!AJ8+Chemicals!AR8</f>
         <v>41140.488667349156</v>
       </c>
     </row>
@@ -37477,15 +37749,15 @@
         <v>2295.0214693815333</v>
       </c>
       <c r="E9" s="8">
-        <f>'Iron&amp;Steel'!W9+'Non-Ferrous'!AC9+'Non-metallic Minerals'!Z9+'Paper&amp;Pulp'!AF9+Chemicals!AI9</f>
+        <f>'Iron&amp;Steel'!W9+'Non-Ferrous'!AC9+'Non-metallic Minerals'!Z9+'Paper&amp;Pulp'!AF9+Chemicals!AM9</f>
         <v>3883.8708277640003</v>
       </c>
       <c r="F9" s="8">
-        <f>'Iron&amp;Steel'!Z9+'Non-Ferrous'!AF9+'Non-metallic Minerals'!AC9+'Paper&amp;Pulp'!AI9+Chemicals!AM9</f>
+        <f>'Iron&amp;Steel'!Z9+'Non-Ferrous'!AF9+'Non-metallic Minerals'!AC9+'Paper&amp;Pulp'!AI9+Chemicals!AQ9</f>
         <v>664.40329199999996</v>
       </c>
       <c r="G9" s="18">
-        <f>'Iron&amp;Steel'!AA9+'Non-Ferrous'!AG9+'Non-metallic Minerals'!AD9+'Paper&amp;Pulp'!AJ9+Chemicals!AN9</f>
+        <f>'Iron&amp;Steel'!AA9+'Non-Ferrous'!AG9+'Non-metallic Minerals'!AD9+'Paper&amp;Pulp'!AJ9+Chemicals!AR9</f>
         <v>3219.4659437640003</v>
       </c>
     </row>
@@ -37506,15 +37778,15 @@
         <v>1000.2021172927061</v>
       </c>
       <c r="E10" s="8">
-        <f>'Iron&amp;Steel'!W10+'Non-Ferrous'!AC10+'Non-metallic Minerals'!Z10+'Paper&amp;Pulp'!AF10+Chemicals!AI10</f>
+        <f>'Iron&amp;Steel'!W10+'Non-Ferrous'!AC10+'Non-metallic Minerals'!Z10+'Paper&amp;Pulp'!AF10+Chemicals!AM10</f>
         <v>1868.5511978856</v>
       </c>
       <c r="F10" s="8">
-        <f>'Iron&amp;Steel'!Z10+'Non-Ferrous'!AF10+'Non-metallic Minerals'!AC10+'Paper&amp;Pulp'!AI10+Chemicals!AM10</f>
+        <f>'Iron&amp;Steel'!Z10+'Non-Ferrous'!AF10+'Non-metallic Minerals'!AC10+'Paper&amp;Pulp'!AI10+Chemicals!AQ10</f>
         <v>307.14364799999998</v>
       </c>
       <c r="G10" s="18">
-        <f>'Iron&amp;Steel'!AA10+'Non-Ferrous'!AG10+'Non-metallic Minerals'!AD10+'Paper&amp;Pulp'!AJ10+Chemicals!AN10</f>
+        <f>'Iron&amp;Steel'!AA10+'Non-Ferrous'!AG10+'Non-metallic Minerals'!AD10+'Paper&amp;Pulp'!AJ10+Chemicals!AR10</f>
         <v>1561.4056898855999</v>
       </c>
     </row>
@@ -37535,15 +37807,15 @@
         <v>3884.2936574155706</v>
       </c>
       <c r="E11" s="8">
-        <f>'Iron&amp;Steel'!W11+'Non-Ferrous'!AC11+'Non-metallic Minerals'!Z11+'Paper&amp;Pulp'!AF11+Chemicals!AI11</f>
+        <f>'Iron&amp;Steel'!W11+'Non-Ferrous'!AC11+'Non-metallic Minerals'!Z11+'Paper&amp;Pulp'!AF11+Chemicals!AM11</f>
         <v>9443.095404440799</v>
       </c>
       <c r="F11" s="8">
-        <f>'Iron&amp;Steel'!Z11+'Non-Ferrous'!AF11+'Non-metallic Minerals'!AC11+'Paper&amp;Pulp'!AI11+Chemicals!AM11</f>
+        <f>'Iron&amp;Steel'!Z11+'Non-Ferrous'!AF11+'Non-metallic Minerals'!AC11+'Paper&amp;Pulp'!AI11+Chemicals!AQ11</f>
         <v>1220.1172560000002</v>
       </c>
       <c r="G11" s="18">
-        <f>'Iron&amp;Steel'!AA11+'Non-Ferrous'!AG11+'Non-metallic Minerals'!AD11+'Paper&amp;Pulp'!AJ11+Chemicals!AN11</f>
+        <f>'Iron&amp;Steel'!AA11+'Non-Ferrous'!AG11+'Non-metallic Minerals'!AD11+'Paper&amp;Pulp'!AJ11+Chemicals!AR11</f>
         <v>8222.9794764407998</v>
       </c>
     </row>
@@ -37564,15 +37836,15 @@
         <v>1794.5041555520047</v>
       </c>
       <c r="E12" s="8">
-        <f>'Iron&amp;Steel'!W12+'Non-Ferrous'!AC12+'Non-metallic Minerals'!Z12+'Paper&amp;Pulp'!AF12+Chemicals!AI12</f>
+        <f>'Iron&amp;Steel'!W12+'Non-Ferrous'!AC12+'Non-metallic Minerals'!Z12+'Paper&amp;Pulp'!AF12+Chemicals!AM12</f>
         <v>2582.2862087283775</v>
       </c>
       <c r="F12" s="8">
-        <f>'Iron&amp;Steel'!Z12+'Non-Ferrous'!AF12+'Non-metallic Minerals'!AC12+'Paper&amp;Pulp'!AI12+Chemicals!AM12</f>
+        <f>'Iron&amp;Steel'!Z12+'Non-Ferrous'!AF12+'Non-metallic Minerals'!AC12+'Paper&amp;Pulp'!AI12+Chemicals!AQ12</f>
         <v>465.27908400000013</v>
       </c>
       <c r="G12" s="18">
-        <f>'Iron&amp;Steel'!AA12+'Non-Ferrous'!AG12+'Non-metallic Minerals'!AD12+'Paper&amp;Pulp'!AJ12+Chemicals!AN12</f>
+        <f>'Iron&amp;Steel'!AA12+'Non-Ferrous'!AG12+'Non-metallic Minerals'!AD12+'Paper&amp;Pulp'!AJ12+Chemicals!AR12</f>
         <v>2152.6963881731999</v>
       </c>
     </row>
@@ -37593,15 +37865,15 @@
         <v>4857.014802678209</v>
       </c>
       <c r="E13" s="8">
-        <f>'Iron&amp;Steel'!W13+'Non-Ferrous'!AC13+'Non-metallic Minerals'!Z13+'Paper&amp;Pulp'!AF13+Chemicals!AI13</f>
+        <f>'Iron&amp;Steel'!W13+'Non-Ferrous'!AC13+'Non-metallic Minerals'!Z13+'Paper&amp;Pulp'!AF13+Chemicals!AM13</f>
         <v>9428.0054046431505</v>
       </c>
       <c r="F13" s="8">
-        <f>'Iron&amp;Steel'!Z13+'Non-Ferrous'!AF13+'Non-metallic Minerals'!AC13+'Paper&amp;Pulp'!AI13+Chemicals!AM13</f>
+        <f>'Iron&amp;Steel'!Z13+'Non-Ferrous'!AF13+'Non-metallic Minerals'!AC13+'Paper&amp;Pulp'!AI13+Chemicals!AQ13</f>
         <v>1256.5332543439858</v>
       </c>
       <c r="G13" s="18">
-        <f>'Iron&amp;Steel'!AA13+'Non-Ferrous'!AG13+'Non-metallic Minerals'!AD13+'Paper&amp;Pulp'!AJ13+Chemicals!AN13</f>
+        <f>'Iron&amp;Steel'!AA13+'Non-Ferrous'!AG13+'Non-metallic Minerals'!AD13+'Paper&amp;Pulp'!AJ13+Chemicals!AR13</f>
         <v>8471.3883121461313</v>
       </c>
     </row>
@@ -37622,15 +37894,15 @@
         <v>2965.048505576211</v>
       </c>
       <c r="E14" s="8">
-        <f>'Iron&amp;Steel'!W14+'Non-Ferrous'!AC14+'Non-metallic Minerals'!Z14+'Paper&amp;Pulp'!AF14+Chemicals!AI14</f>
+        <f>'Iron&amp;Steel'!W14+'Non-Ferrous'!AC14+'Non-metallic Minerals'!Z14+'Paper&amp;Pulp'!AF14+Chemicals!AM14</f>
         <v>4548.4416545011991</v>
       </c>
       <c r="F14" s="8">
-        <f>'Iron&amp;Steel'!Z14+'Non-Ferrous'!AF14+'Non-metallic Minerals'!AC14+'Paper&amp;Pulp'!AI14+Chemicals!AM14</f>
+        <f>'Iron&amp;Steel'!Z14+'Non-Ferrous'!AF14+'Non-metallic Minerals'!AC14+'Paper&amp;Pulp'!AI14+Chemicals!AQ14</f>
         <v>690.06837600000006</v>
       </c>
       <c r="G14" s="18">
-        <f>'Iron&amp;Steel'!AA14+'Non-Ferrous'!AG14+'Non-metallic Minerals'!AD14+'Paper&amp;Pulp'!AJ14+Chemicals!AN14</f>
+        <f>'Iron&amp;Steel'!AA14+'Non-Ferrous'!AG14+'Non-metallic Minerals'!AD14+'Paper&amp;Pulp'!AJ14+Chemicals!AR14</f>
         <v>3858.3713265012002</v>
       </c>
     </row>
@@ -37651,15 +37923,15 @@
         <v>4073.3901171779517</v>
       </c>
       <c r="E15" s="8">
-        <f>'Iron&amp;Steel'!W15+'Non-Ferrous'!AC15+'Non-metallic Minerals'!Z15+'Paper&amp;Pulp'!AF15+Chemicals!AI15</f>
+        <f>'Iron&amp;Steel'!W15+'Non-Ferrous'!AC15+'Non-metallic Minerals'!Z15+'Paper&amp;Pulp'!AF15+Chemicals!AM15</f>
         <v>7604.9409534157585</v>
       </c>
       <c r="F15" s="8">
-        <f>'Iron&amp;Steel'!Z15+'Non-Ferrous'!AF15+'Non-metallic Minerals'!AC15+'Paper&amp;Pulp'!AI15+Chemicals!AM15</f>
+        <f>'Iron&amp;Steel'!Z15+'Non-Ferrous'!AF15+'Non-metallic Minerals'!AC15+'Paper&amp;Pulp'!AI15+Chemicals!AQ15</f>
         <v>1483.873133591434</v>
       </c>
       <c r="G15" s="18">
-        <f>'Iron&amp;Steel'!AA15+'Non-Ferrous'!AG15+'Non-metallic Minerals'!AD15+'Paper&amp;Pulp'!AJ15+Chemicals!AN15</f>
+        <f>'Iron&amp;Steel'!AA15+'Non-Ferrous'!AG15+'Non-metallic Minerals'!AD15+'Paper&amp;Pulp'!AJ15+Chemicals!AR15</f>
         <v>6442.2375755330704</v>
       </c>
     </row>
@@ -37680,15 +37952,15 @@
         <v>467.89689952663457</v>
       </c>
       <c r="E16" s="8">
-        <f>'Iron&amp;Steel'!W16+'Non-Ferrous'!AC16+'Non-metallic Minerals'!Z16+'Paper&amp;Pulp'!AF16+Chemicals!AI16</f>
+        <f>'Iron&amp;Steel'!W16+'Non-Ferrous'!AC16+'Non-metallic Minerals'!Z16+'Paper&amp;Pulp'!AF16+Chemicals!AM16</f>
         <v>933.95673449668152</v>
       </c>
       <c r="F16" s="8">
-        <f>'Iron&amp;Steel'!Z16+'Non-Ferrous'!AF16+'Non-metallic Minerals'!AC16+'Paper&amp;Pulp'!AI16+Chemicals!AM16</f>
+        <f>'Iron&amp;Steel'!Z16+'Non-Ferrous'!AF16+'Non-metallic Minerals'!AC16+'Paper&amp;Pulp'!AI16+Chemicals!AQ16</f>
         <v>168.05887418109296</v>
       </c>
       <c r="G16" s="18">
-        <f>'Iron&amp;Steel'!AA16+'Non-Ferrous'!AG16+'Non-metallic Minerals'!AD16+'Paper&amp;Pulp'!AJ16+Chemicals!AN16</f>
+        <f>'Iron&amp;Steel'!AA16+'Non-Ferrous'!AG16+'Non-metallic Minerals'!AD16+'Paper&amp;Pulp'!AJ16+Chemicals!AR16</f>
         <v>725.48679691009443</v>
       </c>
     </row>
@@ -37709,15 +37981,15 @@
         <v>3280.8751369504716</v>
       </c>
       <c r="E17" s="8">
-        <f>'Iron&amp;Steel'!W17+'Non-Ferrous'!AC17+'Non-metallic Minerals'!Z17+'Paper&amp;Pulp'!AF17+Chemicals!AI17</f>
+        <f>'Iron&amp;Steel'!W17+'Non-Ferrous'!AC17+'Non-metallic Minerals'!Z17+'Paper&amp;Pulp'!AF17+Chemicals!AM17</f>
         <v>7508.4226909554363</v>
       </c>
       <c r="F17" s="8">
-        <f>'Iron&amp;Steel'!Z17+'Non-Ferrous'!AF17+'Non-metallic Minerals'!AC17+'Paper&amp;Pulp'!AI17+Chemicals!AM17</f>
+        <f>'Iron&amp;Steel'!Z17+'Non-Ferrous'!AF17+'Non-metallic Minerals'!AC17+'Paper&amp;Pulp'!AI17+Chemicals!AQ17</f>
         <v>908.2167393670527</v>
       </c>
       <c r="G17" s="18">
-        <f>'Iron&amp;Steel'!AA17+'Non-Ferrous'!AG17+'Non-metallic Minerals'!AD17+'Paper&amp;Pulp'!AJ17+Chemicals!AN17</f>
+        <f>'Iron&amp;Steel'!AA17+'Non-Ferrous'!AG17+'Non-metallic Minerals'!AD17+'Paper&amp;Pulp'!AJ17+Chemicals!AR17</f>
         <v>6352.4143306049054</v>
       </c>
     </row>
@@ -37738,15 +38010,15 @@
         <v>2086.4936572577935</v>
       </c>
       <c r="E18" s="8">
-        <f>'Iron&amp;Steel'!W18+'Non-Ferrous'!AC18+'Non-metallic Minerals'!Z18+'Paper&amp;Pulp'!AF18+Chemicals!AI18</f>
+        <f>'Iron&amp;Steel'!W18+'Non-Ferrous'!AC18+'Non-metallic Minerals'!Z18+'Paper&amp;Pulp'!AF18+Chemicals!AM18</f>
         <v>3748.1251243607999</v>
       </c>
       <c r="F18" s="8">
-        <f>'Iron&amp;Steel'!Z18+'Non-Ferrous'!AF18+'Non-metallic Minerals'!AC18+'Paper&amp;Pulp'!AI18+Chemicals!AM18</f>
+        <f>'Iron&amp;Steel'!Z18+'Non-Ferrous'!AF18+'Non-metallic Minerals'!AC18+'Paper&amp;Pulp'!AI18+Chemicals!AQ18</f>
         <v>507.23081999999999</v>
       </c>
       <c r="G18" s="18">
-        <f>'Iron&amp;Steel'!AA18+'Non-Ferrous'!AG18+'Non-metallic Minerals'!AD18+'Paper&amp;Pulp'!AJ18+Chemicals!AN18</f>
+        <f>'Iron&amp;Steel'!AA18+'Non-Ferrous'!AG18+'Non-metallic Minerals'!AD18+'Paper&amp;Pulp'!AJ18+Chemicals!AR18</f>
         <v>4172.7348700012953</v>
       </c>
     </row>
@@ -37767,15 +38039,15 @@
         <v>7216.7780677552673</v>
       </c>
       <c r="E19" s="8">
-        <f>'Iron&amp;Steel'!W19+'Non-Ferrous'!AC19+'Non-metallic Minerals'!Z19+'Paper&amp;Pulp'!AF19+Chemicals!AI19</f>
+        <f>'Iron&amp;Steel'!W19+'Non-Ferrous'!AC19+'Non-metallic Minerals'!Z19+'Paper&amp;Pulp'!AF19+Chemicals!AM19</f>
         <v>11871.947035580002</v>
       </c>
       <c r="F19" s="8">
-        <f>'Iron&amp;Steel'!Z19+'Non-Ferrous'!AF19+'Non-metallic Minerals'!AC19+'Paper&amp;Pulp'!AI19+Chemicals!AM19</f>
+        <f>'Iron&amp;Steel'!Z19+'Non-Ferrous'!AF19+'Non-metallic Minerals'!AC19+'Paper&amp;Pulp'!AI19+Chemicals!AQ19</f>
         <v>1356.2775018935249</v>
       </c>
       <c r="G19" s="18">
-        <f>'Iron&amp;Steel'!AA19+'Non-Ferrous'!AG19+'Non-metallic Minerals'!AD19+'Paper&amp;Pulp'!AJ19+Chemicals!AN19</f>
+        <f>'Iron&amp;Steel'!AA19+'Non-Ferrous'!AG19+'Non-metallic Minerals'!AD19+'Paper&amp;Pulp'!AJ19+Chemicals!AR19</f>
         <v>10675.99186758</v>
       </c>
     </row>
@@ -37796,15 +38068,15 @@
         <v>4860.7567361617621</v>
       </c>
       <c r="E20" s="22">
-        <f>'Iron&amp;Steel'!W20+'Non-Ferrous'!AC20+'Non-metallic Minerals'!Z20+'Paper&amp;Pulp'!AF20+Chemicals!AI20</f>
+        <f>'Iron&amp;Steel'!W20+'Non-Ferrous'!AC20+'Non-metallic Minerals'!Z20+'Paper&amp;Pulp'!AF20+Chemicals!AM20</f>
         <v>7415.9717279999995</v>
       </c>
       <c r="F20" s="22">
-        <f>'Iron&amp;Steel'!Z20+'Non-Ferrous'!AF20+'Non-metallic Minerals'!AC20+'Paper&amp;Pulp'!AI20+Chemicals!AM20</f>
+        <f>'Iron&amp;Steel'!Z20+'Non-Ferrous'!AF20+'Non-metallic Minerals'!AC20+'Paper&amp;Pulp'!AI20+Chemicals!AQ20</f>
         <v>1467.5152679999999</v>
       </c>
       <c r="G20" s="23">
-        <f>'Iron&amp;Steel'!AA20+'Non-Ferrous'!AG20+'Non-metallic Minerals'!AD20+'Paper&amp;Pulp'!AJ20+Chemicals!AN20</f>
+        <f>'Iron&amp;Steel'!AA20+'Non-Ferrous'!AG20+'Non-metallic Minerals'!AD20+'Paper&amp;Pulp'!AJ20+Chemicals!AR20</f>
         <v>6009.1046510250917</v>
       </c>
     </row>
@@ -37838,24 +38110,24 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B1" s="265" t="s">
+      <c r="B1" s="264" t="s">
         <v>85</v>
       </c>
-      <c r="C1" s="266"/>
-      <c r="D1" s="266"/>
-      <c r="E1" s="266"/>
-      <c r="F1" s="266"/>
-      <c r="G1" s="266"/>
-      <c r="H1" s="267"/>
-      <c r="I1" s="265" t="s">
+      <c r="C1" s="265"/>
+      <c r="D1" s="265"/>
+      <c r="E1" s="265"/>
+      <c r="F1" s="265"/>
+      <c r="G1" s="265"/>
+      <c r="H1" s="266"/>
+      <c r="I1" s="264" t="s">
         <v>86</v>
       </c>
-      <c r="J1" s="266"/>
-      <c r="K1" s="266"/>
-      <c r="L1" s="266"/>
-      <c r="M1" s="266"/>
-      <c r="N1" s="266"/>
-      <c r="O1" s="267"/>
+      <c r="J1" s="265"/>
+      <c r="K1" s="265"/>
+      <c r="L1" s="265"/>
+      <c r="M1" s="265"/>
+      <c r="N1" s="265"/>
+      <c r="O1" s="266"/>
     </row>
     <row r="2" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="9"/>
@@ -37923,7 +38195,7 @@
         <v>1.4273682256151674</v>
       </c>
       <c r="F3" s="74">
-        <f>Chemicals!Z8</f>
+        <f>Chemicals!AB8</f>
         <v>1.056757863096452</v>
       </c>
       <c r="G3" s="55">
@@ -37984,7 +38256,7 @@
         <v>1.4273682256151674</v>
       </c>
       <c r="F4" s="75">
-        <f>Chemicals!Z5</f>
+        <f>Chemicals!AB5</f>
         <v>1.1220004789136599</v>
       </c>
       <c r="G4" s="55">
@@ -38045,7 +38317,7 @@
         <v>1.8562440667081421</v>
       </c>
       <c r="F5" s="75">
-        <f>Chemicals!Z7</f>
+        <f>Chemicals!AB7</f>
         <v>1.1305288523279819</v>
       </c>
       <c r="G5" s="55">
@@ -38106,7 +38378,7 @@
         <v>1.1231715589481093</v>
       </c>
       <c r="F6" s="75">
-        <f>Chemicals!Z12</f>
+        <f>Chemicals!AB12</f>
         <v>1.2797422273384271</v>
       </c>
       <c r="G6" s="55">
@@ -38167,7 +38439,7 @@
         <v>1.3097038287095204</v>
       </c>
       <c r="F7" s="75">
-        <f>Chemicals!Z20</f>
+        <f>Chemicals!AB20</f>
         <v>1.147653479937246</v>
       </c>
       <c r="G7" s="55">
@@ -38228,7 +38500,7 @@
         <v>1.3149409145252782</v>
       </c>
       <c r="F8" s="75">
-        <f>Chemicals!Z9</f>
+        <f>Chemicals!AB9</f>
         <v>1.5131725796500084</v>
       </c>
       <c r="G8" s="55">
@@ -38289,7 +38561,7 @@
         <v>1.169394302396437</v>
       </c>
       <c r="F9" s="75">
-        <f>Chemicals!Z14</f>
+        <f>Chemicals!AB14</f>
         <v>1.5864008837502654</v>
       </c>
       <c r="G9" s="55">
@@ -38350,7 +38622,7 @@
         <v>1.7572352899319701</v>
       </c>
       <c r="F10" s="75">
-        <f>Chemicals!Z15</f>
+        <f>Chemicals!AB15</f>
         <v>1.5445884513002417</v>
       </c>
       <c r="G10" s="55">
@@ -38411,7 +38683,7 @@
         <v>1.4273682256151674</v>
       </c>
       <c r="F11" s="75">
-        <f>Chemicals!Z13</f>
+        <f>Chemicals!AB13</f>
         <v>1.6145656785206102</v>
       </c>
       <c r="G11" s="55">
@@ -38472,7 +38744,7 @@
         <v>1.4273682256151674</v>
       </c>
       <c r="F12" s="75">
-        <f>Chemicals!Z16</f>
+        <f>Chemicals!AB16</f>
         <v>2.4882252747336446</v>
       </c>
       <c r="G12" s="55">
@@ -38533,7 +38805,7 @@
         <v>1.4396214796950364</v>
       </c>
       <c r="F13" s="75">
-        <f>Chemicals!Z10</f>
+        <f>Chemicals!AB10</f>
         <v>1.8082052518661162</v>
       </c>
       <c r="G13" s="55">
@@ -38594,7 +38866,7 @@
         <v>1.4273682256151674</v>
       </c>
       <c r="F14" s="75">
-        <f>Chemicals!Z17</f>
+        <f>Chemicals!AB17</f>
         <v>2.8033372539248047</v>
       </c>
       <c r="G14" s="55">
@@ -38655,7 +38927,7 @@
         <v>1.5592322627054462</v>
       </c>
       <c r="F15" s="75">
-        <f>Chemicals!Z11</f>
+        <f>Chemicals!AB11</f>
         <v>2.27075364854243</v>
       </c>
       <c r="G15" s="55">
@@ -38716,7 +38988,7 @@
         <v>1.4273682256151674</v>
       </c>
       <c r="F16" s="75">
-        <f>Chemicals!Z6</f>
+        <f>Chemicals!AB6</f>
         <v>1.6206123181197565</v>
       </c>
       <c r="G16" s="55">
@@ -38777,7 +39049,7 @@
         <v>1.539879471150889</v>
       </c>
       <c r="F17" s="75">
-        <f>Chemicals!Z19</f>
+        <f>Chemicals!AB19</f>
         <v>1.4023615353766246</v>
       </c>
       <c r="G17" s="55">
@@ -38838,7 +39110,7 @@
         <v>1.2042590813808476</v>
       </c>
       <c r="F18" s="77">
-        <f>Chemicals!Z18</f>
+        <f>Chemicals!AB18</f>
         <v>2.1045803101102205</v>
       </c>
       <c r="G18" s="57">
@@ -38926,13 +39198,13 @@
       <c r="H22" s="8"/>
     </row>
     <row r="23" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B23" s="268"/>
-      <c r="C23" s="268"/>
-      <c r="D23" s="268"/>
-      <c r="E23" s="268"/>
-      <c r="F23" s="268"/>
-      <c r="G23" s="268"/>
-      <c r="H23" s="268"/>
+      <c r="B23" s="267"/>
+      <c r="C23" s="267"/>
+      <c r="D23" s="267"/>
+      <c r="E23" s="267"/>
+      <c r="F23" s="267"/>
+      <c r="G23" s="267"/>
+      <c r="H23" s="267"/>
     </row>
     <row r="25" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A25" s="59"/>

</xml_diff>